<commit_message>
fixed the convergence problem on the J1 feeder.  GridLAB-D solution still not good for J1
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee123x.xlsx
+++ b/CPYDAR/ieee123x.xlsx
@@ -15744,13 +15744,13 @@
         </is>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S21" t="n">
         <v>-16</v>
@@ -15918,7 +15918,7 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q23" t="n">
         <v>0</v>
@@ -15997,7 +15997,7 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Q24" t="n">
         <v>0</v>
@@ -16155,7 +16155,7 @@
         </is>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -16313,7 +16313,7 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q28" t="n">
         <v>0</v>
@@ -36481,7 +36481,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1_C</t>
+          <t>1_B</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -36496,7 +36496,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -36507,7 +36507,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1_A</t>
+          <t>1_C</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -36522,7 +36522,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -36533,7 +36533,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1_B</t>
+          <t>1_A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -36548,7 +36548,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -36585,7 +36585,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>100_C</t>
+          <t>100_B</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -36600,7 +36600,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -36611,7 +36611,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>100_A</t>
+          <t>100_C</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -36626,7 +36626,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -36637,7 +36637,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>100_B</t>
+          <t>100_A</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -36652,7 +36652,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -36663,7 +36663,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>101_C</t>
+          <t>101_B</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -36678,7 +36678,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -36689,7 +36689,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>101_A</t>
+          <t>101_C</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -36704,7 +36704,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -36715,7 +36715,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>101_B</t>
+          <t>101_A</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -36730,7 +36730,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -36819,7 +36819,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>105_C</t>
+          <t>105_B</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -36834,7 +36834,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -36845,7 +36845,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>105_A</t>
+          <t>105_C</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -36860,7 +36860,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -36871,7 +36871,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>105_B</t>
+          <t>105_A</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -36886,7 +36886,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -36949,7 +36949,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>108_C</t>
+          <t>108_B</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -36964,7 +36964,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -36975,7 +36975,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>108_A</t>
+          <t>108_C</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -36990,7 +36990,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -37001,7 +37001,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>108_B</t>
+          <t>108_A</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -37016,7 +37016,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -37235,7 +37235,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13_C</t>
+          <t>13_B</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -37250,7 +37250,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -37261,7 +37261,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13_A</t>
+          <t>13_C</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -37276,7 +37276,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -37287,7 +37287,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13_B</t>
+          <t>13_A</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -37302,7 +37302,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -37313,7 +37313,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>135_C</t>
+          <t>135_B</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -37328,7 +37328,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -37339,7 +37339,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>135_A</t>
+          <t>135_C</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -37354,7 +37354,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -37365,7 +37365,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>135_B</t>
+          <t>135_A</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -37380,7 +37380,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -37417,7 +37417,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>149_C</t>
+          <t>149_B</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -37432,7 +37432,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -37443,7 +37443,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>149_A</t>
+          <t>149_C</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -37458,7 +37458,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -37469,7 +37469,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>149_B</t>
+          <t>149_A</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -37484,7 +37484,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -37521,7 +37521,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>150_C</t>
+          <t>150_B</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -37536,7 +37536,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -37547,7 +37547,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>150_A</t>
+          <t>150_C</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -37562,7 +37562,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -37573,7 +37573,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>150_B</t>
+          <t>150_A</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -37588,7 +37588,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -37599,7 +37599,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>150r_C</t>
+          <t>150r_B</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -37614,7 +37614,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -37625,7 +37625,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>150r_A</t>
+          <t>150r_C</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -37640,7 +37640,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -37651,7 +37651,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>150r_B</t>
+          <t>150r_A</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -37666,7 +37666,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -37677,7 +37677,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>151_C</t>
+          <t>151_B</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -37692,7 +37692,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -37703,7 +37703,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>151_A</t>
+          <t>151_C</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -37718,7 +37718,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -37729,7 +37729,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>151_B</t>
+          <t>151_A</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -37744,7 +37744,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -37755,7 +37755,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>152_C</t>
+          <t>152_B</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -37770,7 +37770,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -37781,7 +37781,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>152_A</t>
+          <t>152_C</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -37796,7 +37796,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -37807,7 +37807,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>152_B</t>
+          <t>152_A</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -37822,7 +37822,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -37859,7 +37859,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>160_C</t>
+          <t>160_B</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -37874,7 +37874,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -37885,7 +37885,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>160_A</t>
+          <t>160_C</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -37900,7 +37900,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -37911,7 +37911,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>160_B</t>
+          <t>160_A</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -37926,7 +37926,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -37937,7 +37937,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>160r_C</t>
+          <t>160r_B</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -37952,7 +37952,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -37963,7 +37963,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>160r_A</t>
+          <t>160r_C</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -37978,7 +37978,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -37989,7 +37989,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>160r_B</t>
+          <t>160r_A</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -38004,7 +38004,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -38041,7 +38041,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>18_C</t>
+          <t>18_B</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -38056,7 +38056,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -38067,7 +38067,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>18_A</t>
+          <t>18_C</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -38082,7 +38082,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -38093,7 +38093,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>18_B</t>
+          <t>18_A</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -38108,7 +38108,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -38145,7 +38145,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>197_C</t>
+          <t>197_B</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -38160,7 +38160,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -38171,7 +38171,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>197_A</t>
+          <t>197_C</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -38186,7 +38186,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -38197,7 +38197,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>197_B</t>
+          <t>197_A</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -38212,7 +38212,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -38275,7 +38275,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>21_C</t>
+          <t>21_B</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -38290,7 +38290,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -38301,7 +38301,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21_A</t>
+          <t>21_C</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -38316,7 +38316,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -38327,7 +38327,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>21_B</t>
+          <t>21_A</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -38342,7 +38342,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -38379,7 +38379,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>23_C</t>
+          <t>23_B</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -38394,7 +38394,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -38405,7 +38405,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>23_A</t>
+          <t>23_C</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -38420,7 +38420,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -38431,7 +38431,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>23_B</t>
+          <t>23_A</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -38446,7 +38446,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -38483,7 +38483,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>25_C</t>
+          <t>25_B</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -38498,7 +38498,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -38509,7 +38509,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>25_A</t>
+          <t>25_C</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -38524,7 +38524,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -38535,7 +38535,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>25_B</t>
+          <t>25_A</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -38550,7 +38550,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -38561,7 +38561,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>250_C</t>
+          <t>250_B</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -38576,7 +38576,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -38587,7 +38587,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>250_A</t>
+          <t>250_C</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -38602,7 +38602,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -38613,7 +38613,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>250_B</t>
+          <t>250_A</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -38628,7 +38628,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -38795,7 +38795,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>28_C</t>
+          <t>28_B</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -38810,7 +38810,7 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -38821,7 +38821,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>28_A</t>
+          <t>28_C</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -38836,7 +38836,7 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -38847,7 +38847,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>28_B</t>
+          <t>28_A</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -38862,7 +38862,7 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -38873,7 +38873,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>29_C</t>
+          <t>29_B</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -38888,7 +38888,7 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -38899,7 +38899,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>29_A</t>
+          <t>29_C</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -38914,7 +38914,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -38925,7 +38925,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>29_B</t>
+          <t>29_A</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -38940,7 +38940,7 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -38977,7 +38977,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>30_C</t>
+          <t>30_B</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -38992,7 +38992,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -39003,7 +39003,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>30_A</t>
+          <t>30_C</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -39018,7 +39018,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -39029,7 +39029,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>30_B</t>
+          <t>30_A</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -39044,7 +39044,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -39055,7 +39055,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>300_C</t>
+          <t>300_B</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -39070,7 +39070,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -39081,7 +39081,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>300_A</t>
+          <t>300_C</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -39096,7 +39096,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -39107,7 +39107,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>300_B</t>
+          <t>300_A</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -39122,7 +39122,7 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -39133,7 +39133,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>300_open_C</t>
+          <t>300_open_B</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -39148,7 +39148,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -39159,7 +39159,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>300_open_A</t>
+          <t>300_open_C</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -39174,7 +39174,7 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -39185,7 +39185,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>300_open_B</t>
+          <t>300_open_A</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -39200,7 +39200,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -39315,7 +39315,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>35_C</t>
+          <t>35_B</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -39330,7 +39330,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -39341,7 +39341,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>35_A</t>
+          <t>35_C</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -39356,7 +39356,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -39367,7 +39367,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>35_B</t>
+          <t>35_A</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -39382,7 +39382,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -39393,7 +39393,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>36_A</t>
+          <t>36_B</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -39408,7 +39408,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -39419,7 +39419,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>36_B</t>
+          <t>36_A</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -39434,7 +39434,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -39549,7 +39549,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>40_C</t>
+          <t>40_B</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -39564,7 +39564,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -39575,7 +39575,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>40_A</t>
+          <t>40_C</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -39590,7 +39590,7 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -39601,7 +39601,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>40_B</t>
+          <t>40_A</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -39616,7 +39616,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -39653,7 +39653,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>42_C</t>
+          <t>42_B</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -39668,7 +39668,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
@@ -39679,7 +39679,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>42_A</t>
+          <t>42_C</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -39694,7 +39694,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -39705,7 +39705,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>42_B</t>
+          <t>42_A</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -39720,7 +39720,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -39757,7 +39757,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>44_C</t>
+          <t>44_B</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -39772,7 +39772,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -39783,7 +39783,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>44_A</t>
+          <t>44_C</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -39798,7 +39798,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -39809,7 +39809,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>44_B</t>
+          <t>44_A</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -39824,7 +39824,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -39861,7 +39861,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>450_C</t>
+          <t>450_B</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -39876,7 +39876,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -39887,7 +39887,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>450_A</t>
+          <t>450_C</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -39902,7 +39902,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -39913,7 +39913,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>450_B</t>
+          <t>450_A</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -39928,7 +39928,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -39965,7 +39965,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>47_C</t>
+          <t>47_B</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -39980,7 +39980,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -39991,7 +39991,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>47_A</t>
+          <t>47_C</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -40006,7 +40006,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -40017,7 +40017,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>47_B</t>
+          <t>47_A</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -40032,7 +40032,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -40043,7 +40043,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>48_C</t>
+          <t>48_B</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -40058,7 +40058,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -40069,7 +40069,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>48_A</t>
+          <t>48_C</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -40084,7 +40084,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -40095,7 +40095,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>48_B</t>
+          <t>48_A</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -40110,7 +40110,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -40121,7 +40121,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>49_C</t>
+          <t>49_B</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -40136,7 +40136,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -40147,7 +40147,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>49_A</t>
+          <t>49_C</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -40162,7 +40162,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -40173,7 +40173,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>49_B</t>
+          <t>49_A</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -40188,7 +40188,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -40225,7 +40225,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>50_C</t>
+          <t>50_B</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -40240,7 +40240,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -40251,7 +40251,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>50_A</t>
+          <t>50_C</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -40266,7 +40266,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -40277,7 +40277,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>50_B</t>
+          <t>50_A</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -40292,7 +40292,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -40303,7 +40303,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>51_C</t>
+          <t>51_B</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -40318,7 +40318,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -40329,7 +40329,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>51_A</t>
+          <t>51_C</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -40344,7 +40344,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -40355,7 +40355,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>51_B</t>
+          <t>51_A</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -40370,7 +40370,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -40381,7 +40381,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>52_C</t>
+          <t>52_B</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -40396,7 +40396,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -40407,7 +40407,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>52_A</t>
+          <t>52_C</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -40422,7 +40422,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -40433,7 +40433,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>52_B</t>
+          <t>52_A</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -40448,7 +40448,7 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -40459,7 +40459,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>53_C</t>
+          <t>53_B</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -40474,7 +40474,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -40485,7 +40485,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>53_A</t>
+          <t>53_C</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -40500,7 +40500,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -40511,7 +40511,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>53_B</t>
+          <t>53_A</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -40526,7 +40526,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -40537,7 +40537,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>54_C</t>
+          <t>54_B</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -40552,7 +40552,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -40563,7 +40563,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>54_A</t>
+          <t>54_C</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -40578,7 +40578,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -40589,7 +40589,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>54_B</t>
+          <t>54_A</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -40604,7 +40604,7 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -40615,7 +40615,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>55_C</t>
+          <t>55_B</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -40630,7 +40630,7 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
@@ -40641,7 +40641,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>55_A</t>
+          <t>55_C</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -40656,7 +40656,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -40667,7 +40667,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>55_B</t>
+          <t>55_A</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -40682,7 +40682,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -40693,7 +40693,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>56_C</t>
+          <t>56_B</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -40708,7 +40708,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -40719,7 +40719,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>56_A</t>
+          <t>56_C</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -40734,7 +40734,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
@@ -40745,7 +40745,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>56_B</t>
+          <t>56_A</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -40760,7 +40760,7 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
@@ -40771,7 +40771,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>57_C</t>
+          <t>57_B</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -40786,7 +40786,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -40797,7 +40797,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>57_A</t>
+          <t>57_C</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -40812,7 +40812,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -40823,7 +40823,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>57_B</t>
+          <t>57_A</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -40838,7 +40838,7 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -40927,7 +40927,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>60_C</t>
+          <t>60_B</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -40942,7 +40942,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -40953,7 +40953,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>60_A</t>
+          <t>60_C</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -40968,7 +40968,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
@@ -40979,7 +40979,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>60_B</t>
+          <t>60_A</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -40994,7 +40994,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -41005,7 +41005,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>61_C</t>
+          <t>61_B</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -41020,7 +41020,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -41031,7 +41031,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>61_A</t>
+          <t>61_C</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -41046,7 +41046,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
@@ -41057,7 +41057,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>61_B</t>
+          <t>61_A</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -41072,7 +41072,7 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -41083,7 +41083,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>610_C</t>
+          <t>610_B</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -41098,7 +41098,7 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
@@ -41109,7 +41109,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>610_A</t>
+          <t>610_C</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -41124,7 +41124,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -41135,7 +41135,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>610_B</t>
+          <t>610_A</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -41150,7 +41150,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
@@ -41161,7 +41161,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>61s_C</t>
+          <t>61s_B</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -41176,7 +41176,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -41187,7 +41187,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>61s_A</t>
+          <t>61s_C</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -41202,7 +41202,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -41213,7 +41213,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>61s_B</t>
+          <t>61s_A</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -41228,7 +41228,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -41239,7 +41239,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>62_C</t>
+          <t>62_B</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -41254,7 +41254,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -41265,7 +41265,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>62_A</t>
+          <t>62_C</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -41280,7 +41280,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -41291,7 +41291,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>62_B</t>
+          <t>62_A</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -41306,7 +41306,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -41317,7 +41317,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>63_C</t>
+          <t>63_B</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -41332,7 +41332,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -41343,7 +41343,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>63_A</t>
+          <t>63_C</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -41358,7 +41358,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -41369,7 +41369,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>63_B</t>
+          <t>63_A</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -41384,7 +41384,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -41395,7 +41395,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>64_C</t>
+          <t>64_B</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -41410,7 +41410,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -41421,7 +41421,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>64_A</t>
+          <t>64_C</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -41436,7 +41436,7 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -41447,7 +41447,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>64_B</t>
+          <t>64_A</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -41462,7 +41462,7 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -41473,7 +41473,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>65_C</t>
+          <t>65_B</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -41488,7 +41488,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -41499,7 +41499,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>65_A</t>
+          <t>65_C</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -41514,7 +41514,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
@@ -41525,7 +41525,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>65_B</t>
+          <t>65_A</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -41540,7 +41540,7 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -41551,7 +41551,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>66_C</t>
+          <t>66_B</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -41566,7 +41566,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -41577,7 +41577,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>66_A</t>
+          <t>66_C</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -41592,7 +41592,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -41603,7 +41603,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>66_B</t>
+          <t>66_A</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -41618,7 +41618,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -41629,7 +41629,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>67_C</t>
+          <t>67_B</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -41644,7 +41644,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -41655,7 +41655,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>67_A</t>
+          <t>67_C</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -41670,7 +41670,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -41681,7 +41681,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>67_B</t>
+          <t>67_A</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -41696,7 +41696,7 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -41759,7 +41759,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>7_C</t>
+          <t>7_B</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -41774,7 +41774,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -41785,7 +41785,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>7_A</t>
+          <t>7_C</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -41800,7 +41800,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -41811,7 +41811,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>7_B</t>
+          <t>7_A</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -41826,7 +41826,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -41889,7 +41889,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>72_C</t>
+          <t>72_B</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -41904,7 +41904,7 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -41915,7 +41915,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>72_A</t>
+          <t>72_C</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -41930,7 +41930,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -41941,7 +41941,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>72_B</t>
+          <t>72_A</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -41956,7 +41956,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -42045,7 +42045,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>76_C</t>
+          <t>76_B</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -42060,7 +42060,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -42071,7 +42071,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>76_A</t>
+          <t>76_C</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -42086,7 +42086,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
@@ -42097,7 +42097,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>76_B</t>
+          <t>76_A</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -42112,7 +42112,7 @@
         </is>
       </c>
       <c r="E218" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
@@ -42123,7 +42123,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>77_C</t>
+          <t>77_B</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -42138,7 +42138,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
@@ -42149,7 +42149,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>77_A</t>
+          <t>77_C</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -42164,7 +42164,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -42175,7 +42175,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>77_B</t>
+          <t>77_A</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -42190,7 +42190,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F221" t="inlineStr">
         <is>
@@ -42201,7 +42201,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>78_C</t>
+          <t>78_B</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -42216,7 +42216,7 @@
         </is>
       </c>
       <c r="E222" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
@@ -42227,7 +42227,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>78_A</t>
+          <t>78_C</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -42242,7 +42242,7 @@
         </is>
       </c>
       <c r="E223" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -42253,7 +42253,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>78_B</t>
+          <t>78_A</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -42268,7 +42268,7 @@
         </is>
       </c>
       <c r="E224" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F224" t="inlineStr">
         <is>
@@ -42279,7 +42279,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>79_C</t>
+          <t>79_B</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -42294,7 +42294,7 @@
         </is>
       </c>
       <c r="E225" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
@@ -42305,7 +42305,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>79_A</t>
+          <t>79_C</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -42320,7 +42320,7 @@
         </is>
       </c>
       <c r="E226" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F226" t="inlineStr">
         <is>
@@ -42331,7 +42331,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>79_B</t>
+          <t>79_A</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -42346,7 +42346,7 @@
         </is>
       </c>
       <c r="E227" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F227" t="inlineStr">
         <is>
@@ -42357,7 +42357,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>8_C</t>
+          <t>8_B</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -42372,7 +42372,7 @@
         </is>
       </c>
       <c r="E228" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -42383,7 +42383,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>8_A</t>
+          <t>8_C</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -42398,7 +42398,7 @@
         </is>
       </c>
       <c r="E229" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
@@ -42409,7 +42409,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>8_B</t>
+          <t>8_A</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -42424,7 +42424,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
@@ -42435,7 +42435,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>80_C</t>
+          <t>80_B</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -42450,7 +42450,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>
@@ -42461,7 +42461,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>80_A</t>
+          <t>80_C</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -42476,7 +42476,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
@@ -42487,7 +42487,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>80_B</t>
+          <t>80_A</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -42502,7 +42502,7 @@
         </is>
       </c>
       <c r="E233" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F233" t="inlineStr">
         <is>
@@ -42513,7 +42513,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>81_C</t>
+          <t>81_B</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -42528,7 +42528,7 @@
         </is>
       </c>
       <c r="E234" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F234" t="inlineStr">
         <is>
@@ -42539,7 +42539,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>81_A</t>
+          <t>81_C</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -42554,7 +42554,7 @@
         </is>
       </c>
       <c r="E235" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F235" t="inlineStr">
         <is>
@@ -42565,7 +42565,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>81_B</t>
+          <t>81_A</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -42580,7 +42580,7 @@
         </is>
       </c>
       <c r="E236" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
@@ -42591,7 +42591,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>82_C</t>
+          <t>82_B</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -42606,7 +42606,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
@@ -42617,7 +42617,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>82_A</t>
+          <t>82_C</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -42632,7 +42632,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
@@ -42643,7 +42643,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>82_B</t>
+          <t>82_A</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -42658,7 +42658,7 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F239" t="inlineStr">
         <is>
@@ -42669,7 +42669,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>83_C</t>
+          <t>83_B</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -42684,7 +42684,7 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -42695,7 +42695,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>83_A</t>
+          <t>83_C</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -42710,7 +42710,7 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -42721,7 +42721,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>83_B</t>
+          <t>83_A</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -42736,7 +42736,7 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F242" t="inlineStr">
         <is>
@@ -42799,7 +42799,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>86_C</t>
+          <t>86_B</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -42814,7 +42814,7 @@
         </is>
       </c>
       <c r="E245" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -42825,7 +42825,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>86_A</t>
+          <t>86_C</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -42840,7 +42840,7 @@
         </is>
       </c>
       <c r="E246" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -42851,7 +42851,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>86_B</t>
+          <t>86_A</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -42866,7 +42866,7 @@
         </is>
       </c>
       <c r="E247" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F247" t="inlineStr">
         <is>
@@ -42877,7 +42877,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>87_C</t>
+          <t>87_B</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -42892,7 +42892,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
@@ -42903,7 +42903,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>87_A</t>
+          <t>87_C</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -42918,7 +42918,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F249" t="inlineStr">
         <is>
@@ -42929,7 +42929,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>87_B</t>
+          <t>87_A</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -42944,7 +42944,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F250" t="inlineStr">
         <is>
@@ -42981,7 +42981,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>89_C</t>
+          <t>89_B</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -42996,7 +42996,7 @@
         </is>
       </c>
       <c r="E252" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -43007,7 +43007,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>89_A</t>
+          <t>89_C</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -43022,7 +43022,7 @@
         </is>
       </c>
       <c r="E253" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F253" t="inlineStr">
         <is>
@@ -43033,7 +43033,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>89_B</t>
+          <t>89_A</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -43048,7 +43048,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F254" t="inlineStr">
         <is>
@@ -43111,7 +43111,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>91_C</t>
+          <t>91_B</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -43126,7 +43126,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F257" t="inlineStr">
         <is>
@@ -43137,7 +43137,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>91_A</t>
+          <t>91_C</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -43152,7 +43152,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F258" t="inlineStr">
         <is>
@@ -43163,7 +43163,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>91_B</t>
+          <t>91_A</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -43178,7 +43178,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F259" t="inlineStr">
         <is>
@@ -43215,7 +43215,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>93_C</t>
+          <t>93_B</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -43230,7 +43230,7 @@
         </is>
       </c>
       <c r="E261" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F261" t="inlineStr">
         <is>
@@ -43241,7 +43241,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>93_A</t>
+          <t>93_C</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -43256,7 +43256,7 @@
         </is>
       </c>
       <c r="E262" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F262" t="inlineStr">
         <is>
@@ -43267,7 +43267,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>93_B</t>
+          <t>93_A</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -43282,7 +43282,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
@@ -43345,7 +43345,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>95_C</t>
+          <t>95_B</t>
         </is>
       </c>
       <c r="B266" t="n">
@@ -43360,7 +43360,7 @@
         </is>
       </c>
       <c r="E266" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F266" t="inlineStr">
         <is>
@@ -43371,7 +43371,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>95_A</t>
+          <t>95_C</t>
         </is>
       </c>
       <c r="B267" t="n">
@@ -43386,7 +43386,7 @@
         </is>
       </c>
       <c r="E267" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F267" t="inlineStr">
         <is>
@@ -43397,7 +43397,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>95_B</t>
+          <t>95_A</t>
         </is>
       </c>
       <c r="B268" t="n">
@@ -43412,7 +43412,7 @@
         </is>
       </c>
       <c r="E268" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
@@ -43449,7 +43449,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>97_C</t>
+          <t>97_B</t>
         </is>
       </c>
       <c r="B270" t="n">
@@ -43464,7 +43464,7 @@
         </is>
       </c>
       <c r="E270" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -43475,7 +43475,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>97_A</t>
+          <t>97_C</t>
         </is>
       </c>
       <c r="B271" t="n">
@@ -43490,7 +43490,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F271" t="inlineStr">
         <is>
@@ -43501,7 +43501,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>97_B</t>
+          <t>97_A</t>
         </is>
       </c>
       <c r="B272" t="n">
@@ -43516,7 +43516,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F272" t="inlineStr">
         <is>
@@ -43527,7 +43527,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>98_C</t>
+          <t>98_B</t>
         </is>
       </c>
       <c r="B273" t="n">
@@ -43542,7 +43542,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
@@ -43553,7 +43553,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>98_A</t>
+          <t>98_C</t>
         </is>
       </c>
       <c r="B274" t="n">
@@ -43568,7 +43568,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F274" t="inlineStr">
         <is>
@@ -43579,7 +43579,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>98_B</t>
+          <t>98_A</t>
         </is>
       </c>
       <c r="B275" t="n">
@@ -43594,7 +43594,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F275" t="inlineStr">
         <is>
@@ -43605,7 +43605,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>99_C</t>
+          <t>99_B</t>
         </is>
       </c>
       <c r="B276" t="n">
@@ -43620,7 +43620,7 @@
         </is>
       </c>
       <c r="E276" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -43631,7 +43631,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>99_A</t>
+          <t>99_C</t>
         </is>
       </c>
       <c r="B277" t="n">
@@ -43646,7 +43646,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F277" t="inlineStr">
         <is>
@@ -43657,7 +43657,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>99_B</t>
+          <t>99_A</t>
         </is>
       </c>
       <c r="B278" t="n">
@@ -43672,7 +43672,7 @@
         </is>
       </c>
       <c r="E278" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update ePHASORSIM for GMDM profile; fixed GLM tank phasing
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee123x.xlsx
+++ b/CPYDAR/ieee123x.xlsx
@@ -1286,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D32" t="n">
         <v>0.12</v>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D33" t="n">
         <v>0.12</v>
@@ -1374,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D34" t="n">
         <v>0.12</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D35" t="n">
         <v>0.12</v>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D36" t="n">
         <v>0.12</v>
@@ -1506,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D37" t="n">
         <v>0.12</v>
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D38" t="n">
         <v>0.12</v>
@@ -1594,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D39" t="n">
         <v>0.12</v>
@@ -1638,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D40" t="n">
         <v>0.12</v>
@@ -1682,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D41" t="n">
         <v>0.12</v>
@@ -1726,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D42" t="n">
         <v>0.12</v>
@@ -1770,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D43" t="n">
         <v>0.12</v>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D44" t="n">
         <v>0.12</v>
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>2.4</v>
+        <v>4.1569219</v>
       </c>
       <c r="D45" t="n">
         <v>0.12</v>
@@ -36481,7 +36481,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1_B</t>
+          <t>1_A</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -36496,7 +36496,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -36507,7 +36507,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1_C</t>
+          <t>1_B</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -36522,7 +36522,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -36533,7 +36533,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1_A</t>
+          <t>1_C</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -36548,7 +36548,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -36585,7 +36585,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>100_B</t>
+          <t>100_A</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -36600,7 +36600,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -36611,7 +36611,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>100_C</t>
+          <t>100_B</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -36626,7 +36626,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -36637,7 +36637,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>100_A</t>
+          <t>100_C</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -36652,7 +36652,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -36663,7 +36663,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>101_B</t>
+          <t>101_A</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -36678,7 +36678,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -36689,7 +36689,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>101_C</t>
+          <t>101_B</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -36704,7 +36704,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -36715,7 +36715,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>101_A</t>
+          <t>101_C</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -36730,7 +36730,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -36819,7 +36819,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>105_B</t>
+          <t>105_A</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -36834,7 +36834,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -36845,7 +36845,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>105_C</t>
+          <t>105_B</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -36860,7 +36860,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -36871,7 +36871,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>105_A</t>
+          <t>105_C</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -36886,7 +36886,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -36949,7 +36949,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>108_B</t>
+          <t>108_A</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -36964,7 +36964,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -36975,7 +36975,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>108_C</t>
+          <t>108_B</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -36990,7 +36990,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -37001,7 +37001,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>108_A</t>
+          <t>108_C</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -37016,7 +37016,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -37235,7 +37235,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>13_B</t>
+          <t>13_A</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -37250,7 +37250,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -37261,7 +37261,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>13_C</t>
+          <t>13_B</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -37276,7 +37276,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -37287,7 +37287,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>13_A</t>
+          <t>13_C</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -37302,7 +37302,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -37313,7 +37313,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>135_B</t>
+          <t>135_A</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -37328,7 +37328,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -37339,7 +37339,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>135_C</t>
+          <t>135_B</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -37354,7 +37354,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -37365,7 +37365,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>135_A</t>
+          <t>135_C</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -37380,7 +37380,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -37417,7 +37417,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>149_B</t>
+          <t>149_A</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -37432,7 +37432,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -37443,7 +37443,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>149_C</t>
+          <t>149_B</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -37458,7 +37458,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -37469,7 +37469,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>149_A</t>
+          <t>149_C</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -37484,7 +37484,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -37521,7 +37521,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>150_B</t>
+          <t>150_A</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -37536,7 +37536,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -37547,7 +37547,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>150_C</t>
+          <t>150_B</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -37562,7 +37562,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -37573,7 +37573,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>150_A</t>
+          <t>150_C</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -37588,7 +37588,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -37599,7 +37599,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>150r_B</t>
+          <t>150r_A</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -37614,7 +37614,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -37625,7 +37625,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>150r_C</t>
+          <t>150r_B</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -37640,7 +37640,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -37651,7 +37651,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>150r_A</t>
+          <t>150r_C</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -37666,7 +37666,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -37677,7 +37677,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>151_B</t>
+          <t>151_A</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -37692,7 +37692,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -37703,7 +37703,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>151_C</t>
+          <t>151_B</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -37718,7 +37718,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -37729,7 +37729,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>151_A</t>
+          <t>151_C</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -37744,7 +37744,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -37755,7 +37755,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>152_B</t>
+          <t>152_A</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -37770,7 +37770,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -37781,7 +37781,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>152_C</t>
+          <t>152_B</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -37796,7 +37796,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -37807,7 +37807,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>152_A</t>
+          <t>152_C</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -37822,7 +37822,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -37859,7 +37859,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>160_B</t>
+          <t>160_A</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -37874,7 +37874,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -37885,7 +37885,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>160_C</t>
+          <t>160_B</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -37900,7 +37900,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -37911,7 +37911,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>160_A</t>
+          <t>160_C</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -37926,7 +37926,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -37937,7 +37937,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>160r_B</t>
+          <t>160r_A</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -37952,7 +37952,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -37963,7 +37963,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>160r_C</t>
+          <t>160r_B</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -37978,7 +37978,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -37989,7 +37989,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>160r_A</t>
+          <t>160r_C</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -38004,7 +38004,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -38041,7 +38041,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>18_B</t>
+          <t>18_A</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -38056,7 +38056,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -38067,7 +38067,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>18_C</t>
+          <t>18_B</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -38082,7 +38082,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -38093,7 +38093,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>18_A</t>
+          <t>18_C</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -38108,7 +38108,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -38145,7 +38145,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>197_B</t>
+          <t>197_A</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -38160,7 +38160,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -38171,7 +38171,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>197_C</t>
+          <t>197_B</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -38186,7 +38186,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -38197,7 +38197,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>197_A</t>
+          <t>197_C</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -38212,7 +38212,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
@@ -38275,7 +38275,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>21_B</t>
+          <t>21_A</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -38290,7 +38290,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -38301,7 +38301,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21_C</t>
+          <t>21_B</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -38316,7 +38316,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -38327,7 +38327,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>21_A</t>
+          <t>21_C</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -38342,7 +38342,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -38379,7 +38379,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>23_B</t>
+          <t>23_A</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -38394,7 +38394,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -38405,7 +38405,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>23_C</t>
+          <t>23_B</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -38420,7 +38420,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -38431,7 +38431,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>23_A</t>
+          <t>23_C</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -38446,7 +38446,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -38483,7 +38483,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>25_B</t>
+          <t>25_A</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -38498,7 +38498,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -38509,7 +38509,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>25_C</t>
+          <t>25_B</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -38524,7 +38524,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -38535,7 +38535,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>25_A</t>
+          <t>25_C</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -38550,7 +38550,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -38561,7 +38561,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>250_B</t>
+          <t>250_A</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -38576,7 +38576,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -38587,7 +38587,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>250_C</t>
+          <t>250_B</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -38602,7 +38602,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -38613,7 +38613,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>250_A</t>
+          <t>250_C</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -38628,7 +38628,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -38639,7 +38639,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>25r_C</t>
+          <t>25r_A</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -38654,7 +38654,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -38665,7 +38665,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>25r_A</t>
+          <t>25r_C</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -38680,7 +38680,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -38691,7 +38691,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>26_C</t>
+          <t>26_A</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -38706,7 +38706,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -38717,7 +38717,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>26_A</t>
+          <t>26_C</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -38732,7 +38732,7 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -38743,7 +38743,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>27_C</t>
+          <t>27_A</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -38758,7 +38758,7 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -38769,7 +38769,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>27_A</t>
+          <t>27_C</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -38784,7 +38784,7 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -38795,7 +38795,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>28_B</t>
+          <t>28_A</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -38810,7 +38810,7 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -38821,7 +38821,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>28_C</t>
+          <t>28_B</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -38836,7 +38836,7 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -38847,7 +38847,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>28_A</t>
+          <t>28_C</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -38862,7 +38862,7 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -38873,7 +38873,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>29_B</t>
+          <t>29_A</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -38888,7 +38888,7 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -38899,7 +38899,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>29_C</t>
+          <t>29_B</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -38914,7 +38914,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -38925,7 +38925,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>29_A</t>
+          <t>29_C</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -38940,7 +38940,7 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -38977,7 +38977,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>30_B</t>
+          <t>30_A</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -38992,7 +38992,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -39003,7 +39003,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>30_C</t>
+          <t>30_B</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -39018,7 +39018,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -39029,7 +39029,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>30_A</t>
+          <t>30_C</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -39044,7 +39044,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -39055,7 +39055,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>300_B</t>
+          <t>300_A</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -39070,7 +39070,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -39081,7 +39081,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>300_C</t>
+          <t>300_B</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -39096,7 +39096,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -39107,7 +39107,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>300_A</t>
+          <t>300_C</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -39122,7 +39122,7 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -39133,7 +39133,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>300_open_B</t>
+          <t>300_open_A</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -39148,7 +39148,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -39159,7 +39159,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>300_open_C</t>
+          <t>300_open_B</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -39174,7 +39174,7 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -39185,7 +39185,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>300_open_A</t>
+          <t>300_open_C</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -39200,7 +39200,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
@@ -39315,7 +39315,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>35_B</t>
+          <t>35_A</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -39330,7 +39330,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -39341,7 +39341,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>35_C</t>
+          <t>35_B</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -39356,7 +39356,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -39367,7 +39367,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>35_A</t>
+          <t>35_C</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -39382,7 +39382,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -39393,7 +39393,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>36_B</t>
+          <t>36_A</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -39408,7 +39408,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -39419,7 +39419,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>36_A</t>
+          <t>36_B</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -39434,7 +39434,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -39549,7 +39549,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>40_B</t>
+          <t>40_A</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -39564,7 +39564,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -39575,7 +39575,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>40_C</t>
+          <t>40_B</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -39590,7 +39590,7 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -39601,7 +39601,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>40_A</t>
+          <t>40_C</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -39616,7 +39616,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -39653,7 +39653,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>42_B</t>
+          <t>42_A</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -39668,7 +39668,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
@@ -39679,7 +39679,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>42_C</t>
+          <t>42_B</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -39694,7 +39694,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -39705,7 +39705,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>42_A</t>
+          <t>42_C</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -39720,7 +39720,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -39757,7 +39757,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>44_B</t>
+          <t>44_A</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -39772,7 +39772,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -39783,7 +39783,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>44_C</t>
+          <t>44_B</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -39798,7 +39798,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -39809,7 +39809,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>44_A</t>
+          <t>44_C</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -39824,7 +39824,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -39861,7 +39861,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>450_B</t>
+          <t>450_A</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -39876,7 +39876,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -39887,7 +39887,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>450_C</t>
+          <t>450_B</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -39902,7 +39902,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -39913,7 +39913,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>450_A</t>
+          <t>450_C</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -39928,7 +39928,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -39965,7 +39965,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>47_B</t>
+          <t>47_A</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -39980,7 +39980,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -39991,7 +39991,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>47_C</t>
+          <t>47_B</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -40006,7 +40006,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -40017,7 +40017,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>47_A</t>
+          <t>47_C</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -40032,7 +40032,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -40043,7 +40043,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>48_B</t>
+          <t>48_A</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -40058,7 +40058,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -40069,7 +40069,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>48_C</t>
+          <t>48_B</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -40084,7 +40084,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -40095,7 +40095,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>48_A</t>
+          <t>48_C</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -40110,7 +40110,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -40121,7 +40121,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>49_B</t>
+          <t>49_A</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -40136,7 +40136,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -40147,7 +40147,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>49_C</t>
+          <t>49_B</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -40162,7 +40162,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -40173,7 +40173,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>49_A</t>
+          <t>49_C</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -40188,7 +40188,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -40225,7 +40225,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>50_B</t>
+          <t>50_A</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -40240,7 +40240,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -40251,7 +40251,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>50_C</t>
+          <t>50_B</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -40266,7 +40266,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -40277,7 +40277,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>50_A</t>
+          <t>50_C</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -40292,7 +40292,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -40303,7 +40303,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>51_B</t>
+          <t>51_A</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -40318,7 +40318,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -40329,7 +40329,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>51_C</t>
+          <t>51_B</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -40344,7 +40344,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -40355,7 +40355,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>51_A</t>
+          <t>51_C</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -40370,7 +40370,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -40381,7 +40381,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>52_B</t>
+          <t>52_A</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -40396,7 +40396,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -40407,7 +40407,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>52_C</t>
+          <t>52_B</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -40422,7 +40422,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -40433,7 +40433,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>52_A</t>
+          <t>52_C</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -40448,7 +40448,7 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -40459,7 +40459,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>53_B</t>
+          <t>53_A</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -40474,7 +40474,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -40485,7 +40485,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>53_C</t>
+          <t>53_B</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -40500,7 +40500,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -40511,7 +40511,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>53_A</t>
+          <t>53_C</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -40526,7 +40526,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -40537,7 +40537,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>54_B</t>
+          <t>54_A</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -40552,7 +40552,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -40563,7 +40563,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>54_C</t>
+          <t>54_B</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -40578,7 +40578,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -40589,7 +40589,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>54_A</t>
+          <t>54_C</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -40604,7 +40604,7 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F160" t="inlineStr">
         <is>
@@ -40615,7 +40615,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>55_B</t>
+          <t>55_A</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -40630,7 +40630,7 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
@@ -40641,7 +40641,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>55_C</t>
+          <t>55_B</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -40656,7 +40656,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -40667,7 +40667,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>55_A</t>
+          <t>55_C</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -40682,7 +40682,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -40693,7 +40693,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>56_B</t>
+          <t>56_A</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -40708,7 +40708,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -40719,7 +40719,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>56_C</t>
+          <t>56_B</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -40734,7 +40734,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
@@ -40745,7 +40745,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>56_A</t>
+          <t>56_C</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -40760,7 +40760,7 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
@@ -40771,7 +40771,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>57_B</t>
+          <t>57_A</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -40786,7 +40786,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -40797,7 +40797,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>57_C</t>
+          <t>57_B</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -40812,7 +40812,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -40823,7 +40823,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>57_A</t>
+          <t>57_C</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -40838,7 +40838,7 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -40927,7 +40927,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>60_B</t>
+          <t>60_A</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -40942,7 +40942,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -40953,7 +40953,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>60_C</t>
+          <t>60_B</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -40968,7 +40968,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
@@ -40979,7 +40979,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>60_A</t>
+          <t>60_C</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -40994,7 +40994,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -41005,7 +41005,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>61_B</t>
+          <t>61_A</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -41020,7 +41020,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -41031,7 +41031,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>61_C</t>
+          <t>61_B</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -41046,7 +41046,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
@@ -41057,7 +41057,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>61_A</t>
+          <t>61_C</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -41072,7 +41072,7 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -41083,7 +41083,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>610_B</t>
+          <t>610_A</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -41098,7 +41098,7 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
@@ -41109,7 +41109,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>610_C</t>
+          <t>610_B</t>
         </is>
       </c>
       <c r="B180" t="n">
@@ -41124,7 +41124,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -41135,7 +41135,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>610_A</t>
+          <t>610_C</t>
         </is>
       </c>
       <c r="B181" t="n">
@@ -41150,7 +41150,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F181" t="inlineStr">
         <is>
@@ -41161,7 +41161,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>61s_B</t>
+          <t>61s_A</t>
         </is>
       </c>
       <c r="B182" t="n">
@@ -41176,7 +41176,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -41187,7 +41187,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>61s_C</t>
+          <t>61s_B</t>
         </is>
       </c>
       <c r="B183" t="n">
@@ -41202,7 +41202,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -41213,7 +41213,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>61s_A</t>
+          <t>61s_C</t>
         </is>
       </c>
       <c r="B184" t="n">
@@ -41228,7 +41228,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -41239,7 +41239,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>62_B</t>
+          <t>62_A</t>
         </is>
       </c>
       <c r="B185" t="n">
@@ -41254,7 +41254,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -41265,7 +41265,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>62_C</t>
+          <t>62_B</t>
         </is>
       </c>
       <c r="B186" t="n">
@@ -41280,7 +41280,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -41291,7 +41291,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>62_A</t>
+          <t>62_C</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -41306,7 +41306,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -41317,7 +41317,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>63_B</t>
+          <t>63_A</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -41332,7 +41332,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -41343,7 +41343,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>63_C</t>
+          <t>63_B</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -41358,7 +41358,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -41369,7 +41369,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>63_A</t>
+          <t>63_C</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -41384,7 +41384,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -41395,7 +41395,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>64_B</t>
+          <t>64_A</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -41410,7 +41410,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -41421,7 +41421,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>64_C</t>
+          <t>64_B</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -41436,7 +41436,7 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -41447,7 +41447,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>64_A</t>
+          <t>64_C</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -41462,7 +41462,7 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -41473,7 +41473,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>65_B</t>
+          <t>65_A</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -41488,7 +41488,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -41499,7 +41499,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>65_C</t>
+          <t>65_B</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -41514,7 +41514,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
@@ -41525,7 +41525,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>65_A</t>
+          <t>65_C</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -41540,7 +41540,7 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -41551,7 +41551,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>66_B</t>
+          <t>66_A</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -41566,7 +41566,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -41577,7 +41577,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>66_C</t>
+          <t>66_B</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -41592,7 +41592,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -41603,7 +41603,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>66_A</t>
+          <t>66_C</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -41618,7 +41618,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -41629,7 +41629,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>67_B</t>
+          <t>67_A</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -41644,7 +41644,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -41655,7 +41655,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>67_C</t>
+          <t>67_B</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -41670,7 +41670,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -41681,7 +41681,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>67_A</t>
+          <t>67_C</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -41696,7 +41696,7 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -41759,7 +41759,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>7_B</t>
+          <t>7_A</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -41774,7 +41774,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -41785,7 +41785,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>7_C</t>
+          <t>7_B</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -41800,7 +41800,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -41811,7 +41811,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>7_A</t>
+          <t>7_C</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -41826,7 +41826,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -41889,7 +41889,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>72_B</t>
+          <t>72_A</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -41904,7 +41904,7 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -41915,7 +41915,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>72_C</t>
+          <t>72_B</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -41930,7 +41930,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -41941,7 +41941,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>72_A</t>
+          <t>72_C</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -41956,7 +41956,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -42045,7 +42045,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>76_B</t>
+          <t>76_A</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -42060,7 +42060,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -42071,7 +42071,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>76_C</t>
+          <t>76_B</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -42086,7 +42086,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
@@ -42097,7 +42097,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>76_A</t>
+          <t>76_C</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -42112,7 +42112,7 @@
         </is>
       </c>
       <c r="E218" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F218" t="inlineStr">
         <is>
@@ -42123,7 +42123,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>77_B</t>
+          <t>77_A</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -42138,7 +42138,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
@@ -42149,7 +42149,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>77_C</t>
+          <t>77_B</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -42164,7 +42164,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F220" t="inlineStr">
         <is>
@@ -42175,7 +42175,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>77_A</t>
+          <t>77_C</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -42190,7 +42190,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F221" t="inlineStr">
         <is>
@@ -42201,7 +42201,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>78_B</t>
+          <t>78_A</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -42216,7 +42216,7 @@
         </is>
       </c>
       <c r="E222" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F222" t="inlineStr">
         <is>
@@ -42227,7 +42227,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>78_C</t>
+          <t>78_B</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -42242,7 +42242,7 @@
         </is>
       </c>
       <c r="E223" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -42253,7 +42253,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>78_A</t>
+          <t>78_C</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -42268,7 +42268,7 @@
         </is>
       </c>
       <c r="E224" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F224" t="inlineStr">
         <is>
@@ -42279,7 +42279,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>79_B</t>
+          <t>79_A</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -42294,7 +42294,7 @@
         </is>
       </c>
       <c r="E225" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F225" t="inlineStr">
         <is>
@@ -42305,7 +42305,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>79_C</t>
+          <t>79_B</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -42320,7 +42320,7 @@
         </is>
       </c>
       <c r="E226" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F226" t="inlineStr">
         <is>
@@ -42331,7 +42331,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>79_A</t>
+          <t>79_C</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -42346,7 +42346,7 @@
         </is>
       </c>
       <c r="E227" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F227" t="inlineStr">
         <is>
@@ -42357,7 +42357,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>8_B</t>
+          <t>8_A</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -42372,7 +42372,7 @@
         </is>
       </c>
       <c r="E228" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -42383,7 +42383,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>8_C</t>
+          <t>8_B</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -42398,7 +42398,7 @@
         </is>
       </c>
       <c r="E229" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
@@ -42409,7 +42409,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>8_A</t>
+          <t>8_C</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -42424,7 +42424,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
@@ -42435,7 +42435,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>80_B</t>
+          <t>80_A</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -42450,7 +42450,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F231" t="inlineStr">
         <is>
@@ -42461,7 +42461,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>80_C</t>
+          <t>80_B</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -42476,7 +42476,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F232" t="inlineStr">
         <is>
@@ -42487,7 +42487,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>80_A</t>
+          <t>80_C</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -42502,7 +42502,7 @@
         </is>
       </c>
       <c r="E233" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F233" t="inlineStr">
         <is>
@@ -42513,7 +42513,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>81_B</t>
+          <t>81_A</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -42528,7 +42528,7 @@
         </is>
       </c>
       <c r="E234" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F234" t="inlineStr">
         <is>
@@ -42539,7 +42539,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>81_C</t>
+          <t>81_B</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -42554,7 +42554,7 @@
         </is>
       </c>
       <c r="E235" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F235" t="inlineStr">
         <is>
@@ -42565,7 +42565,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>81_A</t>
+          <t>81_C</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -42580,7 +42580,7 @@
         </is>
       </c>
       <c r="E236" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
@@ -42591,7 +42591,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>82_B</t>
+          <t>82_A</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -42606,7 +42606,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
@@ -42617,7 +42617,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>82_C</t>
+          <t>82_B</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -42632,7 +42632,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
@@ -42643,7 +42643,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>82_A</t>
+          <t>82_C</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -42658,7 +42658,7 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F239" t="inlineStr">
         <is>
@@ -42669,7 +42669,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>83_B</t>
+          <t>83_A</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -42684,7 +42684,7 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -42695,7 +42695,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>83_C</t>
+          <t>83_B</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -42710,7 +42710,7 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -42721,7 +42721,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>83_A</t>
+          <t>83_C</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -42736,7 +42736,7 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F242" t="inlineStr">
         <is>
@@ -42799,7 +42799,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>86_B</t>
+          <t>86_A</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -42814,7 +42814,7 @@
         </is>
       </c>
       <c r="E245" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -42825,7 +42825,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>86_C</t>
+          <t>86_B</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -42840,7 +42840,7 @@
         </is>
       </c>
       <c r="E246" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -42851,7 +42851,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>86_A</t>
+          <t>86_C</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -42866,7 +42866,7 @@
         </is>
       </c>
       <c r="E247" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F247" t="inlineStr">
         <is>
@@ -42877,7 +42877,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>87_B</t>
+          <t>87_A</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -42892,7 +42892,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
@@ -42903,7 +42903,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>87_C</t>
+          <t>87_B</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -42918,7 +42918,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F249" t="inlineStr">
         <is>
@@ -42929,7 +42929,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>87_A</t>
+          <t>87_C</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -42944,7 +42944,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F250" t="inlineStr">
         <is>
@@ -42981,7 +42981,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>89_B</t>
+          <t>89_A</t>
         </is>
       </c>
       <c r="B252" t="n">
@@ -42996,7 +42996,7 @@
         </is>
       </c>
       <c r="E252" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -43007,7 +43007,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>89_C</t>
+          <t>89_B</t>
         </is>
       </c>
       <c r="B253" t="n">
@@ -43022,7 +43022,7 @@
         </is>
       </c>
       <c r="E253" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F253" t="inlineStr">
         <is>
@@ -43033,7 +43033,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>89_A</t>
+          <t>89_C</t>
         </is>
       </c>
       <c r="B254" t="n">
@@ -43048,7 +43048,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F254" t="inlineStr">
         <is>
@@ -43111,7 +43111,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>91_B</t>
+          <t>91_A</t>
         </is>
       </c>
       <c r="B257" t="n">
@@ -43126,7 +43126,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F257" t="inlineStr">
         <is>
@@ -43137,7 +43137,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>91_C</t>
+          <t>91_B</t>
         </is>
       </c>
       <c r="B258" t="n">
@@ -43152,7 +43152,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F258" t="inlineStr">
         <is>
@@ -43163,7 +43163,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>91_A</t>
+          <t>91_C</t>
         </is>
       </c>
       <c r="B259" t="n">
@@ -43178,7 +43178,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F259" t="inlineStr">
         <is>
@@ -43215,7 +43215,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>93_B</t>
+          <t>93_A</t>
         </is>
       </c>
       <c r="B261" t="n">
@@ -43230,7 +43230,7 @@
         </is>
       </c>
       <c r="E261" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F261" t="inlineStr">
         <is>
@@ -43241,7 +43241,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>93_C</t>
+          <t>93_B</t>
         </is>
       </c>
       <c r="B262" t="n">
@@ -43256,7 +43256,7 @@
         </is>
       </c>
       <c r="E262" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F262" t="inlineStr">
         <is>
@@ -43267,7 +43267,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>93_A</t>
+          <t>93_C</t>
         </is>
       </c>
       <c r="B263" t="n">
@@ -43282,7 +43282,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
@@ -43345,7 +43345,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>95_B</t>
+          <t>95_A</t>
         </is>
       </c>
       <c r="B266" t="n">
@@ -43360,7 +43360,7 @@
         </is>
       </c>
       <c r="E266" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F266" t="inlineStr">
         <is>
@@ -43371,7 +43371,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>95_C</t>
+          <t>95_B</t>
         </is>
       </c>
       <c r="B267" t="n">
@@ -43386,7 +43386,7 @@
         </is>
       </c>
       <c r="E267" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F267" t="inlineStr">
         <is>
@@ -43397,7 +43397,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>95_A</t>
+          <t>95_C</t>
         </is>
       </c>
       <c r="B268" t="n">
@@ -43412,7 +43412,7 @@
         </is>
       </c>
       <c r="E268" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
@@ -43449,7 +43449,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>97_B</t>
+          <t>97_A</t>
         </is>
       </c>
       <c r="B270" t="n">
@@ -43464,7 +43464,7 @@
         </is>
       </c>
       <c r="E270" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -43475,7 +43475,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>97_C</t>
+          <t>97_B</t>
         </is>
       </c>
       <c r="B271" t="n">
@@ -43490,7 +43490,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F271" t="inlineStr">
         <is>
@@ -43501,7 +43501,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>97_A</t>
+          <t>97_C</t>
         </is>
       </c>
       <c r="B272" t="n">
@@ -43516,7 +43516,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F272" t="inlineStr">
         <is>
@@ -43527,7 +43527,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>98_B</t>
+          <t>98_A</t>
         </is>
       </c>
       <c r="B273" t="n">
@@ -43542,7 +43542,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F273" t="inlineStr">
         <is>
@@ -43553,7 +43553,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>98_C</t>
+          <t>98_B</t>
         </is>
       </c>
       <c r="B274" t="n">
@@ -43568,7 +43568,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F274" t="inlineStr">
         <is>
@@ -43579,7 +43579,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>98_A</t>
+          <t>98_C</t>
         </is>
       </c>
       <c r="B275" t="n">
@@ -43594,7 +43594,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F275" t="inlineStr">
         <is>
@@ -43605,7 +43605,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>99_B</t>
+          <t>99_A</t>
         </is>
       </c>
       <c r="B276" t="n">
@@ -43620,7 +43620,7 @@
         </is>
       </c>
       <c r="E276" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -43631,7 +43631,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>99_C</t>
+          <t>99_B</t>
         </is>
       </c>
       <c r="B277" t="n">
@@ -43646,7 +43646,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F277" t="inlineStr">
         <is>
@@ -43657,7 +43657,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>99_A</t>
+          <t>99_C</t>
         </is>
       </c>
       <c r="B278" t="n">
@@ -43672,7 +43672,7 @@
         </is>
       </c>
       <c r="E278" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
regression tests on Windows for 1.0.4
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee123x.xlsx
+++ b/CPYDAR/ieee123x.xlsx
@@ -3282,13 +3282,13 @@
     <t>Unit (V, pu)</t>
   </si>
   <si>
+    <t>300_open_C</t>
+  </si>
+  <si>
+    <t>300_open_A</t>
+  </si>
+  <si>
     <t>300_open_B</t>
-  </si>
-  <si>
-    <t>300_open_C</t>
-  </si>
-  <si>
-    <t>300_open_A</t>
   </si>
   <si>
     <t>94_open_A</t>
@@ -16637,25 +16637,25 @@
         <v>94</v>
       </c>
       <c r="P21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S21">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T21">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U21">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V21">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W21">
         <v>9.999999999999999E-06</v>
@@ -34341,7 +34341,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>479</v>
+        <v>494</v>
       </c>
       <c r="B2">
         <v>2401.777119828843</v>
@@ -34353,7 +34353,7 @@
         <v>1090</v>
       </c>
       <c r="E2">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
         <v>1091</v>
@@ -34361,7 +34361,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>494</v>
+        <v>654</v>
       </c>
       <c r="B3">
         <v>2401.777119828843</v>
@@ -34373,7 +34373,7 @@
         <v>1090</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>1091</v>
@@ -34381,7 +34381,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>654</v>
+        <v>479</v>
       </c>
       <c r="B4">
         <v>2401.777119828843</v>
@@ -34393,7 +34393,7 @@
         <v>1090</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F4" t="s">
         <v>1091</v>
@@ -34421,7 +34421,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>721</v>
+        <v>764</v>
       </c>
       <c r="B6">
         <v>2401.777119828843</v>
@@ -34433,7 +34433,7 @@
         <v>1090</v>
       </c>
       <c r="E6">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
         <v>1091</v>
@@ -34441,7 +34441,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>764</v>
+        <v>681</v>
       </c>
       <c r="B7">
         <v>2401.777119828843</v>
@@ -34453,7 +34453,7 @@
         <v>1090</v>
       </c>
       <c r="E7">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>1091</v>
@@ -34461,7 +34461,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>681</v>
+        <v>721</v>
       </c>
       <c r="B8">
         <v>2401.777119828843</v>
@@ -34473,7 +34473,7 @@
         <v>1090</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F8" t="s">
         <v>1091</v>
@@ -34481,7 +34481,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>682</v>
+        <v>480</v>
       </c>
       <c r="B9">
         <v>2401.777119828843</v>
@@ -34493,7 +34493,7 @@
         <v>1090</v>
       </c>
       <c r="E9">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F9" t="s">
         <v>1091</v>
@@ -34501,7 +34501,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>480</v>
+        <v>643</v>
       </c>
       <c r="B10">
         <v>2401.777119828843</v>
@@ -34513,7 +34513,7 @@
         <v>1090</v>
       </c>
       <c r="E10">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>1091</v>
@@ -34521,7 +34521,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>643</v>
+        <v>682</v>
       </c>
       <c r="B11">
         <v>2401.777119828843</v>
@@ -34533,7 +34533,7 @@
         <v>1090</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F11" t="s">
         <v>1091</v>
@@ -34601,7 +34601,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>483</v>
+        <v>723</v>
       </c>
       <c r="B15">
         <v>2401.777119828843</v>
@@ -34613,7 +34613,7 @@
         <v>1090</v>
       </c>
       <c r="E15">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
         <v>1091</v>
@@ -34621,7 +34621,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>723</v>
+        <v>644</v>
       </c>
       <c r="B16">
         <v>2401.777119828843</v>
@@ -34633,7 +34633,7 @@
         <v>1090</v>
       </c>
       <c r="E16">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>1091</v>
@@ -34641,7 +34641,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>644</v>
+        <v>483</v>
       </c>
       <c r="B17">
         <v>2401.777119828843</v>
@@ -34653,7 +34653,7 @@
         <v>1090</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F17" t="s">
         <v>1091</v>
@@ -34701,7 +34701,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>683</v>
+        <v>724</v>
       </c>
       <c r="B20">
         <v>2401.777119828843</v>
@@ -34713,7 +34713,7 @@
         <v>1090</v>
       </c>
       <c r="E20">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
         <v>1091</v>
@@ -34721,7 +34721,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>724</v>
+        <v>485</v>
       </c>
       <c r="B21">
         <v>2401.777119828843</v>
@@ -34733,7 +34733,7 @@
         <v>1090</v>
       </c>
       <c r="E21">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
         <v>1091</v>
@@ -34741,7 +34741,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>485</v>
+        <v>683</v>
       </c>
       <c r="B22">
         <v>2401.777119828843</v>
@@ -34753,7 +34753,7 @@
         <v>1090</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F22" t="s">
         <v>1091</v>
@@ -34921,7 +34921,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>689</v>
+        <v>490</v>
       </c>
       <c r="B31">
         <v>2401.777119828843</v>
@@ -34933,7 +34933,7 @@
         <v>1090</v>
       </c>
       <c r="E31">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F31" t="s">
         <v>1091</v>
@@ -34941,7 +34941,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>490</v>
+        <v>650</v>
       </c>
       <c r="B32">
         <v>2401.777119828843</v>
@@ -34953,7 +34953,7 @@
         <v>1090</v>
       </c>
       <c r="E32">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F32" t="s">
         <v>1091</v>
@@ -34961,7 +34961,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>650</v>
+        <v>689</v>
       </c>
       <c r="B33">
         <v>2401.777119828843</v>
@@ -34973,7 +34973,7 @@
         <v>1090</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F33" t="s">
         <v>1091</v>
@@ -34981,7 +34981,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>684</v>
+        <v>725</v>
       </c>
       <c r="B34">
         <v>2401.777119828843</v>
@@ -34993,7 +34993,7 @@
         <v>1090</v>
       </c>
       <c r="E34">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F34" t="s">
         <v>1091</v>
@@ -35001,7 +35001,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>725</v>
+        <v>645</v>
       </c>
       <c r="B35">
         <v>2401.777119828843</v>
@@ -35013,7 +35013,7 @@
         <v>1090</v>
       </c>
       <c r="E35">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
         <v>1091</v>
@@ -35021,7 +35021,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>645</v>
+        <v>684</v>
       </c>
       <c r="B36">
         <v>2401.777119828843</v>
@@ -35033,7 +35033,7 @@
         <v>1090</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F36" t="s">
         <v>1091</v>
@@ -35061,7 +35061,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>685</v>
+        <v>726</v>
       </c>
       <c r="B38">
         <v>2401.777119828843</v>
@@ -35073,7 +35073,7 @@
         <v>1090</v>
       </c>
       <c r="E38">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F38" t="s">
         <v>1091</v>
@@ -35081,7 +35081,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>726</v>
+        <v>646</v>
       </c>
       <c r="B39">
         <v>2401.777119828843</v>
@@ -35093,7 +35093,7 @@
         <v>1090</v>
       </c>
       <c r="E39">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F39" t="s">
         <v>1091</v>
@@ -35101,7 +35101,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>646</v>
+        <v>685</v>
       </c>
       <c r="B40">
         <v>2401.777119828843</v>
@@ -35113,7 +35113,7 @@
         <v>1090</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F40" t="s">
         <v>1091</v>
@@ -35141,7 +35141,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>2401.777119828843</v>
@@ -35153,7 +35153,7 @@
         <v>1090</v>
       </c>
       <c r="E42">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
         <v>1092</v>
@@ -35161,7 +35161,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>2401.777119828843</v>
@@ -35173,7 +35173,7 @@
         <v>1090</v>
       </c>
       <c r="E43">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
         <v>1092</v>
@@ -35181,7 +35181,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>2401.777119828843</v>
@@ -35193,7 +35193,7 @@
         <v>1090</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F44" t="s">
         <v>1092</v>
@@ -35201,7 +35201,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B45">
         <v>2401.777119828843</v>
@@ -35213,7 +35213,7 @@
         <v>1090</v>
       </c>
       <c r="E45">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F45" t="s">
         <v>1091</v>
@@ -35221,7 +35221,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="B46">
         <v>2401.777119828843</v>
@@ -35233,7 +35233,7 @@
         <v>1090</v>
       </c>
       <c r="E46">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F46" t="s">
         <v>1091</v>
@@ -35241,7 +35241,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B47">
         <v>2401.777119828843</v>
@@ -35253,7 +35253,7 @@
         <v>1090</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F47" t="s">
         <v>1091</v>
@@ -35261,7 +35261,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="B48">
         <v>2401.777119828843</v>
@@ -35273,7 +35273,7 @@
         <v>1090</v>
       </c>
       <c r="E48">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F48" t="s">
         <v>1091</v>
@@ -35281,7 +35281,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
       <c r="B49">
         <v>2401.777119828843</v>
@@ -35293,7 +35293,7 @@
         <v>1090</v>
       </c>
       <c r="E49">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F49" t="s">
         <v>1091</v>
@@ -35301,7 +35301,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="B50">
         <v>2401.777119828843</v>
@@ -35313,7 +35313,7 @@
         <v>1090</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F50" t="s">
         <v>1091</v>
@@ -35321,7 +35321,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>686</v>
+        <v>727</v>
       </c>
       <c r="B51">
         <v>2401.777119828843</v>
@@ -35333,7 +35333,7 @@
         <v>1090</v>
       </c>
       <c r="E51">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F51" t="s">
         <v>1091</v>
@@ -35341,7 +35341,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>727</v>
+        <v>647</v>
       </c>
       <c r="B52">
         <v>2401.777119828843</v>
@@ -35353,7 +35353,7 @@
         <v>1090</v>
       </c>
       <c r="E52">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
         <v>1091</v>
@@ -35361,7 +35361,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>647</v>
+        <v>686</v>
       </c>
       <c r="B53">
         <v>2401.777119828843</v>
@@ -35373,7 +35373,7 @@
         <v>1090</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F53" t="s">
         <v>1091</v>
@@ -35401,7 +35401,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B55">
         <v>2401.777119828843</v>
@@ -35413,7 +35413,7 @@
         <v>1090</v>
       </c>
       <c r="E55">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F55" t="s">
         <v>1091</v>
@@ -35421,7 +35421,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B56">
         <v>2401.777119828843</v>
@@ -35433,7 +35433,7 @@
         <v>1090</v>
       </c>
       <c r="E56">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F56" t="s">
         <v>1091</v>
@@ -35441,7 +35441,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B57">
         <v>2401.777119828843</v>
@@ -35453,7 +35453,7 @@
         <v>1090</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F57" t="s">
         <v>1091</v>
@@ -35461,7 +35461,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>687</v>
+        <v>728</v>
       </c>
       <c r="B58">
         <v>2401.777119828843</v>
@@ -35473,7 +35473,7 @@
         <v>1090</v>
       </c>
       <c r="E58">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F58" t="s">
         <v>1091</v>
@@ -35481,7 +35481,7 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>728</v>
+        <v>648</v>
       </c>
       <c r="B59">
         <v>2401.777119828843</v>
@@ -35493,7 +35493,7 @@
         <v>1090</v>
       </c>
       <c r="E59">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F59" t="s">
         <v>1091</v>
@@ -35501,7 +35501,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>648</v>
+        <v>687</v>
       </c>
       <c r="B60">
         <v>2401.777119828843</v>
@@ -35513,7 +35513,7 @@
         <v>1090</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F60" t="s">
         <v>1091</v>
@@ -35541,7 +35541,7 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>690</v>
+        <v>730</v>
       </c>
       <c r="B62">
         <v>2401.777119828843</v>
@@ -35553,7 +35553,7 @@
         <v>1090</v>
       </c>
       <c r="E62">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F62" t="s">
         <v>1091</v>
@@ -35561,7 +35561,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>730</v>
+        <v>493</v>
       </c>
       <c r="B63">
         <v>2401.777119828843</v>
@@ -35573,7 +35573,7 @@
         <v>1090</v>
       </c>
       <c r="E63">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F63" t="s">
         <v>1091</v>
@@ -35581,7 +35581,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>493</v>
+        <v>690</v>
       </c>
       <c r="B64">
         <v>2401.777119828843</v>
@@ -35593,7 +35593,7 @@
         <v>1090</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F64" t="s">
         <v>1091</v>
@@ -35621,7 +35621,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>688</v>
+        <v>729</v>
       </c>
       <c r="B66">
         <v>2401.777119828843</v>
@@ -35633,7 +35633,7 @@
         <v>1090</v>
       </c>
       <c r="E66">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F66" t="s">
         <v>1091</v>
@@ -35641,7 +35641,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>729</v>
+        <v>649</v>
       </c>
       <c r="B67">
         <v>2401.777119828843</v>
@@ -35653,7 +35653,7 @@
         <v>1090</v>
       </c>
       <c r="E67">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F67" t="s">
         <v>1091</v>
@@ -35661,7 +35661,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>649</v>
+        <v>688</v>
       </c>
       <c r="B68">
         <v>2401.777119828843</v>
@@ -35673,7 +35673,7 @@
         <v>1090</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F68" t="s">
         <v>1091</v>
@@ -35721,7 +35721,7 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>496</v>
+        <v>731</v>
       </c>
       <c r="B71">
         <v>2401.777119828843</v>
@@ -35733,7 +35733,7 @@
         <v>1090</v>
       </c>
       <c r="E71">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F71" t="s">
         <v>1091</v>
@@ -35741,7 +35741,7 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>731</v>
+        <v>651</v>
       </c>
       <c r="B72">
         <v>2401.777119828843</v>
@@ -35753,7 +35753,7 @@
         <v>1090</v>
       </c>
       <c r="E72">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
         <v>1091</v>
@@ -35761,7 +35761,7 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>651</v>
+        <v>496</v>
       </c>
       <c r="B73">
         <v>2401.777119828843</v>
@@ -35773,7 +35773,7 @@
         <v>1090</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F73" t="s">
         <v>1091</v>
@@ -35801,7 +35801,7 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>691</v>
+        <v>497</v>
       </c>
       <c r="B75">
         <v>2401.777119828843</v>
@@ -35813,7 +35813,7 @@
         <v>1090</v>
       </c>
       <c r="E75">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F75" t="s">
         <v>1091</v>
@@ -35821,7 +35821,7 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>497</v>
+        <v>652</v>
       </c>
       <c r="B76">
         <v>2401.777119828843</v>
@@ -35833,7 +35833,7 @@
         <v>1090</v>
       </c>
       <c r="E76">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F76" t="s">
         <v>1091</v>
@@ -35841,7 +35841,7 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>652</v>
+        <v>691</v>
       </c>
       <c r="B77">
         <v>2401.777119828843</v>
@@ -35853,7 +35853,7 @@
         <v>1090</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F77" t="s">
         <v>1091</v>
@@ -35881,7 +35881,7 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>692</v>
+        <v>732</v>
       </c>
       <c r="B79">
         <v>2401.777119828843</v>
@@ -35893,7 +35893,7 @@
         <v>1090</v>
       </c>
       <c r="E79">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F79" t="s">
         <v>1091</v>
@@ -35901,7 +35901,7 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>732</v>
+        <v>653</v>
       </c>
       <c r="B80">
         <v>2401.777119828843</v>
@@ -35913,7 +35913,7 @@
         <v>1090</v>
       </c>
       <c r="E80">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F80" t="s">
         <v>1091</v>
@@ -35921,7 +35921,7 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>653</v>
+        <v>692</v>
       </c>
       <c r="B81">
         <v>2401.777119828843</v>
@@ -35933,7 +35933,7 @@
         <v>1090</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F81" t="s">
         <v>1091</v>
@@ -35941,7 +35941,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="B82">
         <v>2401.777119828843</v>
@@ -35953,7 +35953,7 @@
         <v>1090</v>
       </c>
       <c r="E82">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F82" t="s">
         <v>1091</v>
@@ -35961,7 +35961,7 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>783</v>
+        <v>766</v>
       </c>
       <c r="B83">
         <v>2401.777119828843</v>
@@ -35973,7 +35973,7 @@
         <v>1090</v>
       </c>
       <c r="E83">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F83" t="s">
         <v>1091</v>
@@ -35981,7 +35981,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="B84">
         <v>2401.777119828843</v>
@@ -35993,7 +35993,7 @@
         <v>1090</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F84" t="s">
         <v>1091</v>
@@ -36121,7 +36121,7 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>693</v>
+        <v>733</v>
       </c>
       <c r="B91">
         <v>2401.777119828843</v>
@@ -36133,7 +36133,7 @@
         <v>1090</v>
       </c>
       <c r="E91">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F91" t="s">
         <v>1091</v>
@@ -36141,7 +36141,7 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>733</v>
+        <v>655</v>
       </c>
       <c r="B92">
         <v>2401.777119828843</v>
@@ -36153,7 +36153,7 @@
         <v>1090</v>
       </c>
       <c r="E92">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F92" t="s">
         <v>1091</v>
@@ -36161,7 +36161,7 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>655</v>
+        <v>693</v>
       </c>
       <c r="B93">
         <v>2401.777119828843</v>
@@ -36173,7 +36173,7 @@
         <v>1090</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F93" t="s">
         <v>1091</v>
@@ -36181,7 +36181,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>694</v>
+        <v>734</v>
       </c>
       <c r="B94">
         <v>2401.777119828843</v>
@@ -36193,7 +36193,7 @@
         <v>1090</v>
       </c>
       <c r="E94">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F94" t="s">
         <v>1091</v>
@@ -36201,7 +36201,7 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>734</v>
+        <v>103</v>
       </c>
       <c r="B95">
         <v>2401.777119828843</v>
@@ -36213,7 +36213,7 @@
         <v>1090</v>
       </c>
       <c r="E95">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F95" t="s">
         <v>1091</v>
@@ -36221,7 +36221,7 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>694</v>
       </c>
       <c r="B96">
         <v>2401.777119828843</v>
@@ -36233,7 +36233,7 @@
         <v>1090</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F96" t="s">
         <v>1091</v>
@@ -36261,7 +36261,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>695</v>
+        <v>735</v>
       </c>
       <c r="B98">
         <v>2401.777119828843</v>
@@ -36273,7 +36273,7 @@
         <v>1090</v>
       </c>
       <c r="E98">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F98" t="s">
         <v>1091</v>
@@ -36281,7 +36281,7 @@
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>735</v>
+        <v>656</v>
       </c>
       <c r="B99">
         <v>2401.777119828843</v>
@@ -36293,7 +36293,7 @@
         <v>1090</v>
       </c>
       <c r="E99">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F99" t="s">
         <v>1091</v>
@@ -36301,7 +36301,7 @@
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>656</v>
+        <v>695</v>
       </c>
       <c r="B100">
         <v>2401.777119828843</v>
@@ -36313,7 +36313,7 @@
         <v>1090</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F100" t="s">
         <v>1091</v>
@@ -36321,7 +36321,7 @@
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>774</v>
+        <v>782</v>
       </c>
       <c r="B101">
         <v>2401.777119828843</v>
@@ -36333,7 +36333,7 @@
         <v>1090</v>
       </c>
       <c r="E101">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F101" t="s">
         <v>1091</v>
@@ -36341,7 +36341,7 @@
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>782</v>
+        <v>765</v>
       </c>
       <c r="B102">
         <v>2401.777119828843</v>
@@ -36353,7 +36353,7 @@
         <v>1090</v>
       </c>
       <c r="E102">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F102" t="s">
         <v>1091</v>
@@ -36361,7 +36361,7 @@
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="B103">
         <v>2401.777119828843</v>
@@ -36373,7 +36373,7 @@
         <v>1090</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F103" t="s">
         <v>1091</v>
@@ -36393,7 +36393,7 @@
         <v>1090</v>
       </c>
       <c r="E104">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F104" t="s">
         <v>1091</v>
@@ -36413,7 +36413,7 @@
         <v>1090</v>
       </c>
       <c r="E105">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F105" t="s">
         <v>1091</v>
@@ -36433,7 +36433,7 @@
         <v>1090</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F106" t="s">
         <v>1091</v>
@@ -36521,7 +36521,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>568</v>
+        <v>736</v>
       </c>
       <c r="B111">
         <v>2401.777119828843</v>
@@ -36533,7 +36533,7 @@
         <v>1090</v>
       </c>
       <c r="E111">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F111" t="s">
         <v>1091</v>
@@ -36541,7 +36541,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>736</v>
+        <v>95</v>
       </c>
       <c r="B112">
         <v>2401.777119828843</v>
@@ -36553,7 +36553,7 @@
         <v>1090</v>
       </c>
       <c r="E112">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F112" t="s">
         <v>1091</v>
@@ -36561,7 +36561,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>95</v>
+        <v>568</v>
       </c>
       <c r="B113">
         <v>2401.777119828843</v>
@@ -36573,7 +36573,7 @@
         <v>1090</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F113" t="s">
         <v>1091</v>
@@ -36581,7 +36581,7 @@
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B114">
         <v>2401.777119828843</v>
@@ -36593,7 +36593,7 @@
         <v>1090</v>
       </c>
       <c r="E114">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F114" t="s">
         <v>1091</v>
@@ -36601,7 +36601,7 @@
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B115">
         <v>2401.777119828843</v>
@@ -36613,7 +36613,7 @@
         <v>1090</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F115" t="s">
         <v>1091</v>
@@ -36701,7 +36701,7 @@
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>696</v>
+        <v>506</v>
       </c>
       <c r="B120">
         <v>2401.777119828843</v>
@@ -36713,7 +36713,7 @@
         <v>1090</v>
       </c>
       <c r="E120">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F120" t="s">
         <v>1091</v>
@@ -36721,7 +36721,7 @@
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>506</v>
+        <v>657</v>
       </c>
       <c r="B121">
         <v>2401.777119828843</v>
@@ -36733,7 +36733,7 @@
         <v>1090</v>
       </c>
       <c r="E121">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F121" t="s">
         <v>1091</v>
@@ -36741,7 +36741,7 @@
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>657</v>
+        <v>696</v>
       </c>
       <c r="B122">
         <v>2401.777119828843</v>
@@ -36753,7 +36753,7 @@
         <v>1090</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F122" t="s">
         <v>1091</v>
@@ -36781,7 +36781,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>507</v>
+        <v>737</v>
       </c>
       <c r="B124">
         <v>2401.777119828843</v>
@@ -36793,7 +36793,7 @@
         <v>1090</v>
       </c>
       <c r="E124">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F124" t="s">
         <v>1091</v>
@@ -36801,7 +36801,7 @@
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>737</v>
+        <v>658</v>
       </c>
       <c r="B125">
         <v>2401.777119828843</v>
@@ -36813,7 +36813,7 @@
         <v>1090</v>
       </c>
       <c r="E125">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F125" t="s">
         <v>1091</v>
@@ -36821,7 +36821,7 @@
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>658</v>
+        <v>507</v>
       </c>
       <c r="B126">
         <v>2401.777119828843</v>
@@ -36833,7 +36833,7 @@
         <v>1090</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F126" t="s">
         <v>1091</v>
@@ -36861,7 +36861,7 @@
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>697</v>
+        <v>738</v>
       </c>
       <c r="B128">
         <v>2401.777119828843</v>
@@ -36873,7 +36873,7 @@
         <v>1090</v>
       </c>
       <c r="E128">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F128" t="s">
         <v>1091</v>
@@ -36881,7 +36881,7 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>738</v>
+        <v>508</v>
       </c>
       <c r="B129">
         <v>2401.777119828843</v>
@@ -36893,7 +36893,7 @@
         <v>1090</v>
       </c>
       <c r="E129">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F129" t="s">
         <v>1091</v>
@@ -36901,7 +36901,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>508</v>
+        <v>697</v>
       </c>
       <c r="B130">
         <v>2401.777119828843</v>
@@ -36913,7 +36913,7 @@
         <v>1090</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F130" t="s">
         <v>1091</v>
@@ -36941,7 +36941,7 @@
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="B132">
         <v>2401.777119828843</v>
@@ -36953,7 +36953,7 @@
         <v>1090</v>
       </c>
       <c r="E132">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F132" t="s">
         <v>1091</v>
@@ -36961,7 +36961,7 @@
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>790</v>
+        <v>773</v>
       </c>
       <c r="B133">
         <v>2401.777119828843</v>
@@ -36973,7 +36973,7 @@
         <v>1090</v>
       </c>
       <c r="E133">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F133" t="s">
         <v>1091</v>
@@ -36981,7 +36981,7 @@
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>773</v>
+        <v>781</v>
       </c>
       <c r="B134">
         <v>2401.777119828843</v>
@@ -36993,7 +36993,7 @@
         <v>1090</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F134" t="s">
         <v>1091</v>
@@ -37021,7 +37021,7 @@
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B136">
         <v>2401.777119828843</v>
@@ -37033,7 +37033,7 @@
         <v>1090</v>
       </c>
       <c r="E136">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F136" t="s">
         <v>1091</v>
@@ -37041,7 +37041,7 @@
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B137">
         <v>2401.777119828843</v>
@@ -37053,7 +37053,7 @@
         <v>1090</v>
       </c>
       <c r="E137">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F137" t="s">
         <v>1091</v>
@@ -37061,7 +37061,7 @@
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B138">
         <v>2401.777119828843</v>
@@ -37073,7 +37073,7 @@
         <v>1090</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F138" t="s">
         <v>1091</v>
@@ -37081,7 +37081,7 @@
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B139">
         <v>2401.777119828843</v>
@@ -37093,7 +37093,7 @@
         <v>1090</v>
       </c>
       <c r="E139">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F139" t="s">
         <v>1091</v>
@@ -37101,7 +37101,7 @@
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B140">
         <v>2401.777119828843</v>
@@ -37113,7 +37113,7 @@
         <v>1090</v>
       </c>
       <c r="E140">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F140" t="s">
         <v>1091</v>
@@ -37121,7 +37121,7 @@
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B141">
         <v>2401.777119828843</v>
@@ -37133,7 +37133,7 @@
         <v>1090</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F141" t="s">
         <v>1091</v>
@@ -37141,7 +37141,7 @@
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>105</v>
+        <v>739</v>
       </c>
       <c r="B142">
         <v>2401.777119828843</v>
@@ -37153,7 +37153,7 @@
         <v>1090</v>
       </c>
       <c r="E142">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F142" t="s">
         <v>1091</v>
@@ -37161,7 +37161,7 @@
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>739</v>
+        <v>659</v>
       </c>
       <c r="B143">
         <v>2401.777119828843</v>
@@ -37173,7 +37173,7 @@
         <v>1090</v>
       </c>
       <c r="E143">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F143" t="s">
         <v>1091</v>
@@ -37181,7 +37181,7 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>659</v>
+        <v>105</v>
       </c>
       <c r="B144">
         <v>2401.777119828843</v>
@@ -37193,7 +37193,7 @@
         <v>1090</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F144" t="s">
         <v>1091</v>
@@ -37221,7 +37221,7 @@
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>698</v>
+        <v>740</v>
       </c>
       <c r="B146">
         <v>2401.777119828843</v>
@@ -37233,7 +37233,7 @@
         <v>1090</v>
       </c>
       <c r="E146">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F146" t="s">
         <v>1091</v>
@@ -37241,7 +37241,7 @@
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>740</v>
+        <v>660</v>
       </c>
       <c r="B147">
         <v>2401.777119828843</v>
@@ -37253,7 +37253,7 @@
         <v>1090</v>
       </c>
       <c r="E147">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F147" t="s">
         <v>1091</v>
@@ -37261,7 +37261,7 @@
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>660</v>
+        <v>698</v>
       </c>
       <c r="B148">
         <v>2401.777119828843</v>
@@ -37273,7 +37273,7 @@
         <v>1090</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F148" t="s">
         <v>1091</v>
@@ -37281,7 +37281,7 @@
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>699</v>
+        <v>741</v>
       </c>
       <c r="B149">
         <v>2401.777119828843</v>
@@ -37293,7 +37293,7 @@
         <v>1090</v>
       </c>
       <c r="E149">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F149" t="s">
         <v>1091</v>
@@ -37301,7 +37301,7 @@
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>741</v>
+        <v>661</v>
       </c>
       <c r="B150">
         <v>2401.777119828843</v>
@@ -37313,7 +37313,7 @@
         <v>1090</v>
       </c>
       <c r="E150">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F150" t="s">
         <v>1091</v>
@@ -37321,7 +37321,7 @@
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>661</v>
+        <v>699</v>
       </c>
       <c r="B151">
         <v>2401.777119828843</v>
@@ -37333,7 +37333,7 @@
         <v>1090</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F151" t="s">
         <v>1091</v>
@@ -37341,7 +37341,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>700</v>
+        <v>742</v>
       </c>
       <c r="B152">
         <v>2401.777119828843</v>
@@ -37353,7 +37353,7 @@
         <v>1090</v>
       </c>
       <c r="E152">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F152" t="s">
         <v>1091</v>
@@ -37361,7 +37361,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>742</v>
+        <v>662</v>
       </c>
       <c r="B153">
         <v>2401.777119828843</v>
@@ -37373,7 +37373,7 @@
         <v>1090</v>
       </c>
       <c r="E153">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F153" t="s">
         <v>1091</v>
@@ -37381,7 +37381,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>662</v>
+        <v>700</v>
       </c>
       <c r="B154">
         <v>2401.777119828843</v>
@@ -37393,7 +37393,7 @@
         <v>1090</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F154" t="s">
         <v>1091</v>
@@ -37401,7 +37401,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>701</v>
+        <v>743</v>
       </c>
       <c r="B155">
         <v>2401.777119828843</v>
@@ -37413,7 +37413,7 @@
         <v>1090</v>
       </c>
       <c r="E155">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F155" t="s">
         <v>1091</v>
@@ -37421,7 +37421,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>743</v>
+        <v>663</v>
       </c>
       <c r="B156">
         <v>2401.777119828843</v>
@@ -37433,7 +37433,7 @@
         <v>1090</v>
       </c>
       <c r="E156">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F156" t="s">
         <v>1091</v>
@@ -37441,7 +37441,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>663</v>
+        <v>701</v>
       </c>
       <c r="B157">
         <v>2401.777119828843</v>
@@ -37453,7 +37453,7 @@
         <v>1090</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F157" t="s">
         <v>1091</v>
@@ -37461,7 +37461,7 @@
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>702</v>
+        <v>744</v>
       </c>
       <c r="B158">
         <v>2401.777119828843</v>
@@ -37473,7 +37473,7 @@
         <v>1090</v>
       </c>
       <c r="E158">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F158" t="s">
         <v>1091</v>
@@ -37481,7 +37481,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>744</v>
+        <v>664</v>
       </c>
       <c r="B159">
         <v>2401.777119828843</v>
@@ -37493,7 +37493,7 @@
         <v>1090</v>
       </c>
       <c r="E159">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F159" t="s">
         <v>1091</v>
@@ -37501,7 +37501,7 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>664</v>
+        <v>702</v>
       </c>
       <c r="B160">
         <v>2401.777119828843</v>
@@ -37513,7 +37513,7 @@
         <v>1090</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F160" t="s">
         <v>1091</v>
@@ -37521,7 +37521,7 @@
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>703</v>
+        <v>745</v>
       </c>
       <c r="B161">
         <v>2401.777119828843</v>
@@ -37533,7 +37533,7 @@
         <v>1090</v>
       </c>
       <c r="E161">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F161" t="s">
         <v>1091</v>
@@ -37541,7 +37541,7 @@
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>745</v>
+        <v>106</v>
       </c>
       <c r="B162">
         <v>2401.777119828843</v>
@@ -37553,7 +37553,7 @@
         <v>1090</v>
       </c>
       <c r="E162">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F162" t="s">
         <v>1091</v>
@@ -37561,7 +37561,7 @@
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>106</v>
+        <v>703</v>
       </c>
       <c r="B163">
         <v>2401.777119828843</v>
@@ -37573,7 +37573,7 @@
         <v>1090</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F163" t="s">
         <v>1091</v>
@@ -37581,7 +37581,7 @@
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>777</v>
+        <v>785</v>
       </c>
       <c r="B164">
         <v>2401.777119828843</v>
@@ -37593,7 +37593,7 @@
         <v>1090</v>
       </c>
       <c r="E164">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F164" t="s">
         <v>1091</v>
@@ -37601,7 +37601,7 @@
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>785</v>
+        <v>768</v>
       </c>
       <c r="B165">
         <v>2401.777119828843</v>
@@ -37613,7 +37613,7 @@
         <v>1090</v>
       </c>
       <c r="E165">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F165" t="s">
         <v>1091</v>
@@ -37621,7 +37621,7 @@
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>768</v>
+        <v>777</v>
       </c>
       <c r="B166">
         <v>2401.777119828843</v>
@@ -37633,7 +37633,7 @@
         <v>1090</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F166" t="s">
         <v>1091</v>
@@ -37641,7 +37641,7 @@
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>510</v>
+        <v>746</v>
       </c>
       <c r="B167">
         <v>2401.777119828843</v>
@@ -37653,7 +37653,7 @@
         <v>1090</v>
       </c>
       <c r="E167">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F167" t="s">
         <v>1091</v>
@@ -37661,7 +37661,7 @@
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>746</v>
+        <v>665</v>
       </c>
       <c r="B168">
         <v>2401.777119828843</v>
@@ -37673,7 +37673,7 @@
         <v>1090</v>
       </c>
       <c r="E168">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F168" t="s">
         <v>1091</v>
@@ -37681,7 +37681,7 @@
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>665</v>
+        <v>510</v>
       </c>
       <c r="B169">
         <v>2401.777119828843</v>
@@ -37693,7 +37693,7 @@
         <v>1090</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F169" t="s">
         <v>1091</v>
@@ -37761,7 +37761,7 @@
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>704</v>
+        <v>747</v>
       </c>
       <c r="B173">
         <v>2401.777119828843</v>
@@ -37773,7 +37773,7 @@
         <v>1090</v>
       </c>
       <c r="E173">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F173" t="s">
         <v>1091</v>
@@ -37781,7 +37781,7 @@
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>747</v>
+        <v>666</v>
       </c>
       <c r="B174">
         <v>2401.777119828843</v>
@@ -37793,7 +37793,7 @@
         <v>1090</v>
       </c>
       <c r="E174">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F174" t="s">
         <v>1091</v>
@@ -37801,7 +37801,7 @@
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>666</v>
+        <v>704</v>
       </c>
       <c r="B175">
         <v>2401.777119828843</v>
@@ -37813,7 +37813,7 @@
         <v>1090</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F175" t="s">
         <v>1091</v>
@@ -37821,7 +37821,7 @@
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>778</v>
+        <v>786</v>
       </c>
       <c r="B176">
         <v>2401.777119828843</v>
@@ -37833,7 +37833,7 @@
         <v>1090</v>
       </c>
       <c r="E176">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F176" t="s">
         <v>1091</v>
@@ -37841,7 +37841,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
       <c r="B177">
         <v>2401.777119828843</v>
@@ -37853,7 +37853,7 @@
         <v>1090</v>
       </c>
       <c r="E177">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F177" t="s">
         <v>1091</v>
@@ -37861,7 +37861,7 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>769</v>
+        <v>778</v>
       </c>
       <c r="B178">
         <v>2401.777119828843</v>
@@ -37873,7 +37873,7 @@
         <v>1090</v>
       </c>
       <c r="E178">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F178" t="s">
         <v>1091</v>
@@ -37881,7 +37881,7 @@
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B179">
         <v>277.1281292110204</v>
@@ -37893,7 +37893,7 @@
         <v>1090</v>
       </c>
       <c r="E179">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F179" t="s">
         <v>1091</v>
@@ -37901,7 +37901,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="B180">
         <v>277.1281292110204</v>
@@ -37913,7 +37913,7 @@
         <v>1090</v>
       </c>
       <c r="E180">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F180" t="s">
         <v>1091</v>
@@ -37921,7 +37921,7 @@
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="B181">
         <v>277.1281292110204</v>
@@ -37933,7 +37933,7 @@
         <v>1090</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F181" t="s">
         <v>1091</v>
@@ -37941,7 +37941,7 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B182">
         <v>2401.777119828843</v>
@@ -37953,7 +37953,7 @@
         <v>1090</v>
       </c>
       <c r="E182">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F182" t="s">
         <v>1091</v>
@@ -37961,7 +37961,7 @@
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
-        <v>1024</v>
+        <v>937</v>
       </c>
       <c r="B183">
         <v>2401.777119828843</v>
@@ -37973,7 +37973,7 @@
         <v>1090</v>
       </c>
       <c r="E183">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F183" t="s">
         <v>1091</v>
@@ -37981,7 +37981,7 @@
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>937</v>
+        <v>1023</v>
       </c>
       <c r="B184">
         <v>2401.777119828843</v>
@@ -37993,7 +37993,7 @@
         <v>1090</v>
       </c>
       <c r="E184">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F184" t="s">
         <v>1091</v>
@@ -38001,7 +38001,7 @@
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
-        <v>705</v>
+        <v>748</v>
       </c>
       <c r="B185">
         <v>2401.777119828843</v>
@@ -38013,7 +38013,7 @@
         <v>1090</v>
       </c>
       <c r="E185">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F185" t="s">
         <v>1091</v>
@@ -38021,7 +38021,7 @@
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>748</v>
+        <v>667</v>
       </c>
       <c r="B186">
         <v>2401.777119828843</v>
@@ -38033,7 +38033,7 @@
         <v>1090</v>
       </c>
       <c r="E186">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F186" t="s">
         <v>1091</v>
@@ -38041,7 +38041,7 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>667</v>
+        <v>705</v>
       </c>
       <c r="B187">
         <v>2401.777119828843</v>
@@ -38053,7 +38053,7 @@
         <v>1090</v>
       </c>
       <c r="E187">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F187" t="s">
         <v>1091</v>
@@ -38061,7 +38061,7 @@
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>706</v>
+        <v>749</v>
       </c>
       <c r="B188">
         <v>2401.777119828843</v>
@@ -38073,7 +38073,7 @@
         <v>1090</v>
       </c>
       <c r="E188">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F188" t="s">
         <v>1091</v>
@@ -38081,7 +38081,7 @@
     </row>
     <row r="189" spans="1:6">
       <c r="A189" t="s">
-        <v>749</v>
+        <v>107</v>
       </c>
       <c r="B189">
         <v>2401.777119828843</v>
@@ -38093,7 +38093,7 @@
         <v>1090</v>
       </c>
       <c r="E189">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F189" t="s">
         <v>1091</v>
@@ -38101,7 +38101,7 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>107</v>
+        <v>706</v>
       </c>
       <c r="B190">
         <v>2401.777119828843</v>
@@ -38113,7 +38113,7 @@
         <v>1090</v>
       </c>
       <c r="E190">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F190" t="s">
         <v>1091</v>
@@ -38121,7 +38121,7 @@
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>707</v>
+        <v>750</v>
       </c>
       <c r="B191">
         <v>2401.777119828843</v>
@@ -38133,7 +38133,7 @@
         <v>1090</v>
       </c>
       <c r="E191">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F191" t="s">
         <v>1091</v>
@@ -38141,7 +38141,7 @@
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>750</v>
+        <v>668</v>
       </c>
       <c r="B192">
         <v>2401.777119828843</v>
@@ -38153,7 +38153,7 @@
         <v>1090</v>
       </c>
       <c r="E192">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F192" t="s">
         <v>1091</v>
@@ -38161,7 +38161,7 @@
     </row>
     <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>668</v>
+        <v>707</v>
       </c>
       <c r="B193">
         <v>2401.777119828843</v>
@@ -38173,7 +38173,7 @@
         <v>1090</v>
       </c>
       <c r="E193">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F193" t="s">
         <v>1091</v>
@@ -38181,7 +38181,7 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B194">
         <v>2401.777119828843</v>
@@ -38193,7 +38193,7 @@
         <v>1090</v>
       </c>
       <c r="E194">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F194" t="s">
         <v>1091</v>
@@ -38201,7 +38201,7 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B195">
         <v>2401.777119828843</v>
@@ -38213,7 +38213,7 @@
         <v>1090</v>
       </c>
       <c r="E195">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F195" t="s">
         <v>1091</v>
@@ -38221,7 +38221,7 @@
     </row>
     <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B196">
         <v>2401.777119828843</v>
@@ -38233,7 +38233,7 @@
         <v>1090</v>
       </c>
       <c r="E196">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F196" t="s">
         <v>1091</v>
@@ -38241,7 +38241,7 @@
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
       <c r="B197">
         <v>2401.777119828843</v>
@@ -38253,7 +38253,7 @@
         <v>1090</v>
       </c>
       <c r="E197">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F197" t="s">
         <v>1091</v>
@@ -38261,7 +38261,7 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
       <c r="B198">
         <v>2401.777119828843</v>
@@ -38273,7 +38273,7 @@
         <v>1090</v>
       </c>
       <c r="E198">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F198" t="s">
         <v>1091</v>
@@ -38281,7 +38281,7 @@
     </row>
     <row r="199" spans="1:6">
       <c r="A199" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="B199">
         <v>2401.777119828843</v>
@@ -38293,7 +38293,7 @@
         <v>1090</v>
       </c>
       <c r="E199">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F199" t="s">
         <v>1091</v>
@@ -38301,7 +38301,7 @@
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>708</v>
+        <v>751</v>
       </c>
       <c r="B200">
         <v>2401.777119828843</v>
@@ -38313,7 +38313,7 @@
         <v>1090</v>
       </c>
       <c r="E200">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F200" t="s">
         <v>1091</v>
@@ -38321,7 +38321,7 @@
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>751</v>
+        <v>513</v>
       </c>
       <c r="B201">
         <v>2401.777119828843</v>
@@ -38333,7 +38333,7 @@
         <v>1090</v>
       </c>
       <c r="E201">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F201" t="s">
         <v>1091</v>
@@ -38341,7 +38341,7 @@
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>513</v>
+        <v>708</v>
       </c>
       <c r="B202">
         <v>2401.777119828843</v>
@@ -38353,7 +38353,7 @@
         <v>1090</v>
       </c>
       <c r="E202">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F202" t="s">
         <v>1091</v>
@@ -38401,7 +38401,7 @@
     </row>
     <row r="205" spans="1:6">
       <c r="A205" t="s">
-        <v>709</v>
+        <v>752</v>
       </c>
       <c r="B205">
         <v>2401.777119828843</v>
@@ -38413,7 +38413,7 @@
         <v>1090</v>
       </c>
       <c r="E205">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F205" t="s">
         <v>1091</v>
@@ -38421,7 +38421,7 @@
     </row>
     <row r="206" spans="1:6">
       <c r="A206" t="s">
-        <v>752</v>
+        <v>109</v>
       </c>
       <c r="B206">
         <v>2401.777119828843</v>
@@ -38433,7 +38433,7 @@
         <v>1090</v>
       </c>
       <c r="E206">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F206" t="s">
         <v>1091</v>
@@ -38441,7 +38441,7 @@
     </row>
     <row r="207" spans="1:6">
       <c r="A207" t="s">
-        <v>109</v>
+        <v>709</v>
       </c>
       <c r="B207">
         <v>2401.777119828843</v>
@@ -38453,7 +38453,7 @@
         <v>1090</v>
       </c>
       <c r="E207">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F207" t="s">
         <v>1091</v>
@@ -38501,7 +38501,7 @@
     </row>
     <row r="210" spans="1:6">
       <c r="A210" t="s">
-        <v>710</v>
+        <v>516</v>
       </c>
       <c r="B210">
         <v>2401.777119828843</v>
@@ -38513,7 +38513,7 @@
         <v>1090</v>
       </c>
       <c r="E210">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F210" t="s">
         <v>1091</v>
@@ -38521,7 +38521,7 @@
     </row>
     <row r="211" spans="1:6">
       <c r="A211" t="s">
-        <v>516</v>
+        <v>669</v>
       </c>
       <c r="B211">
         <v>2401.777119828843</v>
@@ -38533,7 +38533,7 @@
         <v>1090</v>
       </c>
       <c r="E211">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F211" t="s">
         <v>1091</v>
@@ -38541,7 +38541,7 @@
     </row>
     <row r="212" spans="1:6">
       <c r="A212" t="s">
-        <v>669</v>
+        <v>710</v>
       </c>
       <c r="B212">
         <v>2401.777119828843</v>
@@ -38553,7 +38553,7 @@
         <v>1090</v>
       </c>
       <c r="E212">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F212" t="s">
         <v>1091</v>
@@ -38621,7 +38621,7 @@
     </row>
     <row r="216" spans="1:6">
       <c r="A216" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B216">
         <v>2401.777119828843</v>
@@ -38633,7 +38633,7 @@
         <v>1090</v>
       </c>
       <c r="E216">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F216" t="s">
         <v>1091</v>
@@ -38641,7 +38641,7 @@
     </row>
     <row r="217" spans="1:6">
       <c r="A217" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B217">
         <v>2401.777119828843</v>
@@ -38653,7 +38653,7 @@
         <v>1090</v>
       </c>
       <c r="E217">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F217" t="s">
         <v>1091</v>
@@ -38661,7 +38661,7 @@
     </row>
     <row r="218" spans="1:6">
       <c r="A218" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B218">
         <v>2401.777119828843</v>
@@ -38673,7 +38673,7 @@
         <v>1090</v>
       </c>
       <c r="E218">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F218" t="s">
         <v>1091</v>
@@ -38681,7 +38681,7 @@
     </row>
     <row r="219" spans="1:6">
       <c r="A219" t="s">
-        <v>711</v>
+        <v>753</v>
       </c>
       <c r="B219">
         <v>2401.777119828843</v>
@@ -38693,7 +38693,7 @@
         <v>1090</v>
       </c>
       <c r="E219">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F219" t="s">
         <v>1091</v>
@@ -38701,7 +38701,7 @@
     </row>
     <row r="220" spans="1:6">
       <c r="A220" t="s">
-        <v>753</v>
+        <v>670</v>
       </c>
       <c r="B220">
         <v>2401.777119828843</v>
@@ -38713,7 +38713,7 @@
         <v>1090</v>
       </c>
       <c r="E220">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F220" t="s">
         <v>1091</v>
@@ -38721,7 +38721,7 @@
     </row>
     <row r="221" spans="1:6">
       <c r="A221" t="s">
-        <v>670</v>
+        <v>711</v>
       </c>
       <c r="B221">
         <v>2401.777119828843</v>
@@ -38733,7 +38733,7 @@
         <v>1090</v>
       </c>
       <c r="E221">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F221" t="s">
         <v>1091</v>
@@ -38741,7 +38741,7 @@
     </row>
     <row r="222" spans="1:6">
       <c r="A222" t="s">
-        <v>712</v>
+        <v>754</v>
       </c>
       <c r="B222">
         <v>2401.777119828843</v>
@@ -38753,7 +38753,7 @@
         <v>1090</v>
       </c>
       <c r="E222">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F222" t="s">
         <v>1091</v>
@@ -38761,7 +38761,7 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" t="s">
-        <v>754</v>
+        <v>671</v>
       </c>
       <c r="B223">
         <v>2401.777119828843</v>
@@ -38773,7 +38773,7 @@
         <v>1090</v>
       </c>
       <c r="E223">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F223" t="s">
         <v>1091</v>
@@ -38781,7 +38781,7 @@
     </row>
     <row r="224" spans="1:6">
       <c r="A224" t="s">
-        <v>671</v>
+        <v>712</v>
       </c>
       <c r="B224">
         <v>2401.777119828843</v>
@@ -38793,7 +38793,7 @@
         <v>1090</v>
       </c>
       <c r="E224">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F224" t="s">
         <v>1091</v>
@@ -38801,7 +38801,7 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
-        <v>780</v>
+        <v>788</v>
       </c>
       <c r="B225">
         <v>2401.777119828843</v>
@@ -38813,7 +38813,7 @@
         <v>1090</v>
       </c>
       <c r="E225">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F225" t="s">
         <v>1091</v>
@@ -38821,7 +38821,7 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
       <c r="B226">
         <v>2401.777119828843</v>
@@ -38833,7 +38833,7 @@
         <v>1090</v>
       </c>
       <c r="E226">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F226" t="s">
         <v>1091</v>
@@ -38841,7 +38841,7 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="B227">
         <v>2401.777119828843</v>
@@ -38853,7 +38853,7 @@
         <v>1090</v>
       </c>
       <c r="E227">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F227" t="s">
         <v>1091</v>
@@ -38861,7 +38861,7 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" t="s">
-        <v>519</v>
+        <v>722</v>
       </c>
       <c r="B228">
         <v>2401.777119828843</v>
@@ -38873,7 +38873,7 @@
         <v>1090</v>
       </c>
       <c r="E228">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F228" t="s">
         <v>1091</v>
@@ -38881,7 +38881,7 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" t="s">
-        <v>722</v>
+        <v>524</v>
       </c>
       <c r="B229">
         <v>2401.777119828843</v>
@@ -38893,7 +38893,7 @@
         <v>1090</v>
       </c>
       <c r="E229">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F229" t="s">
         <v>1091</v>
@@ -38901,7 +38901,7 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B230">
         <v>2401.777119828843</v>
@@ -38913,7 +38913,7 @@
         <v>1090</v>
       </c>
       <c r="E230">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F230" t="s">
         <v>1091</v>
@@ -38921,7 +38921,7 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" t="s">
-        <v>111</v>
+        <v>755</v>
       </c>
       <c r="B231">
         <v>2401.777119828843</v>
@@ -38933,7 +38933,7 @@
         <v>1090</v>
       </c>
       <c r="E231">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F231" t="s">
         <v>1091</v>
@@ -38941,7 +38941,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" t="s">
-        <v>755</v>
+        <v>672</v>
       </c>
       <c r="B232">
         <v>2401.777119828843</v>
@@ -38953,7 +38953,7 @@
         <v>1090</v>
       </c>
       <c r="E232">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F232" t="s">
         <v>1091</v>
@@ -38961,7 +38961,7 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" t="s">
-        <v>672</v>
+        <v>111</v>
       </c>
       <c r="B233">
         <v>2401.777119828843</v>
@@ -38973,7 +38973,7 @@
         <v>1090</v>
       </c>
       <c r="E233">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F233" t="s">
         <v>1091</v>
@@ -38981,7 +38981,7 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" t="s">
-        <v>713</v>
+        <v>520</v>
       </c>
       <c r="B234">
         <v>2401.777119828843</v>
@@ -38993,7 +38993,7 @@
         <v>1090</v>
       </c>
       <c r="E234">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F234" t="s">
         <v>1091</v>
@@ -39001,7 +39001,7 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" t="s">
-        <v>520</v>
+        <v>673</v>
       </c>
       <c r="B235">
         <v>2401.777119828843</v>
@@ -39013,7 +39013,7 @@
         <v>1090</v>
       </c>
       <c r="E235">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F235" t="s">
         <v>1091</v>
@@ -39021,7 +39021,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" t="s">
-        <v>673</v>
+        <v>713</v>
       </c>
       <c r="B236">
         <v>2401.777119828843</v>
@@ -39033,7 +39033,7 @@
         <v>1090</v>
       </c>
       <c r="E236">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F236" t="s">
         <v>1091</v>
@@ -39041,7 +39041,7 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" t="s">
-        <v>714</v>
+        <v>756</v>
       </c>
       <c r="B237">
         <v>2401.777119828843</v>
@@ -39053,7 +39053,7 @@
         <v>1090</v>
       </c>
       <c r="E237">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F237" t="s">
         <v>1091</v>
@@ -39061,7 +39061,7 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" t="s">
-        <v>756</v>
+        <v>674</v>
       </c>
       <c r="B238">
         <v>2401.777119828843</v>
@@ -39073,7 +39073,7 @@
         <v>1090</v>
       </c>
       <c r="E238">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F238" t="s">
         <v>1091</v>
@@ -39081,7 +39081,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" t="s">
-        <v>674</v>
+        <v>714</v>
       </c>
       <c r="B239">
         <v>2401.777119828843</v>
@@ -39093,7 +39093,7 @@
         <v>1090</v>
       </c>
       <c r="E239">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F239" t="s">
         <v>1091</v>
@@ -39101,7 +39101,7 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B240">
         <v>2401.777119828843</v>
@@ -39113,7 +39113,7 @@
         <v>1090</v>
       </c>
       <c r="E240">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F240" t="s">
         <v>1091</v>
@@ -39121,7 +39121,7 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B241">
         <v>2401.777119828843</v>
@@ -39133,7 +39133,7 @@
         <v>1090</v>
       </c>
       <c r="E241">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F241" t="s">
         <v>1091</v>
@@ -39141,7 +39141,7 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B242">
         <v>2401.777119828843</v>
@@ -39153,7 +39153,7 @@
         <v>1090</v>
       </c>
       <c r="E242">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F242" t="s">
         <v>1091</v>
@@ -39201,7 +39201,7 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" t="s">
-        <v>715</v>
+        <v>757</v>
       </c>
       <c r="B245">
         <v>2401.777119828843</v>
@@ -39213,7 +39213,7 @@
         <v>1090</v>
       </c>
       <c r="E245">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F245" t="s">
         <v>1091</v>
@@ -39221,7 +39221,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" t="s">
-        <v>757</v>
+        <v>675</v>
       </c>
       <c r="B246">
         <v>2401.777119828843</v>
@@ -39233,7 +39233,7 @@
         <v>1090</v>
       </c>
       <c r="E246">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F246" t="s">
         <v>1091</v>
@@ -39241,7 +39241,7 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" t="s">
-        <v>675</v>
+        <v>715</v>
       </c>
       <c r="B247">
         <v>2401.777119828843</v>
@@ -39253,7 +39253,7 @@
         <v>1090</v>
       </c>
       <c r="E247">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F247" t="s">
         <v>1091</v>
@@ -39261,7 +39261,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" t="s">
-        <v>112</v>
+        <v>758</v>
       </c>
       <c r="B248">
         <v>2401.777119828843</v>
@@ -39273,7 +39273,7 @@
         <v>1090</v>
       </c>
       <c r="E248">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F248" t="s">
         <v>1091</v>
@@ -39281,7 +39281,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" t="s">
-        <v>758</v>
+        <v>522</v>
       </c>
       <c r="B249">
         <v>2401.777119828843</v>
@@ -39293,7 +39293,7 @@
         <v>1090</v>
       </c>
       <c r="E249">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F249" t="s">
         <v>1091</v>
@@ -39301,7 +39301,7 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" t="s">
-        <v>522</v>
+        <v>112</v>
       </c>
       <c r="B250">
         <v>2401.777119828843</v>
@@ -39313,7 +39313,7 @@
         <v>1090</v>
       </c>
       <c r="E250">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F250" t="s">
         <v>1091</v>
@@ -39341,7 +39341,7 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" t="s">
-        <v>523</v>
+        <v>759</v>
       </c>
       <c r="B252">
         <v>2401.777119828843</v>
@@ -39353,7 +39353,7 @@
         <v>1090</v>
       </c>
       <c r="E252">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F252" t="s">
         <v>1091</v>
@@ -39361,7 +39361,7 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" t="s">
-        <v>759</v>
+        <v>676</v>
       </c>
       <c r="B253">
         <v>2401.777119828843</v>
@@ -39373,7 +39373,7 @@
         <v>1090</v>
       </c>
       <c r="E253">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F253" t="s">
         <v>1091</v>
@@ -39381,7 +39381,7 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" t="s">
-        <v>676</v>
+        <v>523</v>
       </c>
       <c r="B254">
         <v>2401.777119828843</v>
@@ -39393,7 +39393,7 @@
         <v>1090</v>
       </c>
       <c r="E254">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F254" t="s">
         <v>1091</v>
@@ -39441,7 +39441,7 @@
     </row>
     <row r="257" spans="1:6">
       <c r="A257" t="s">
-        <v>716</v>
+        <v>525</v>
       </c>
       <c r="B257">
         <v>2401.777119828843</v>
@@ -39453,7 +39453,7 @@
         <v>1090</v>
       </c>
       <c r="E257">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F257" t="s">
         <v>1091</v>
@@ -39461,7 +39461,7 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258" t="s">
-        <v>525</v>
+        <v>677</v>
       </c>
       <c r="B258">
         <v>2401.777119828843</v>
@@ -39473,7 +39473,7 @@
         <v>1090</v>
       </c>
       <c r="E258">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F258" t="s">
         <v>1091</v>
@@ -39481,7 +39481,7 @@
     </row>
     <row r="259" spans="1:6">
       <c r="A259" t="s">
-        <v>677</v>
+        <v>716</v>
       </c>
       <c r="B259">
         <v>2401.777119828843</v>
@@ -39493,7 +39493,7 @@
         <v>1090</v>
       </c>
       <c r="E259">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F259" t="s">
         <v>1091</v>
@@ -39521,7 +39521,7 @@
     </row>
     <row r="261" spans="1:6">
       <c r="A261" t="s">
-        <v>717</v>
+        <v>760</v>
       </c>
       <c r="B261">
         <v>2401.777119828843</v>
@@ -39533,7 +39533,7 @@
         <v>1090</v>
       </c>
       <c r="E261">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F261" t="s">
         <v>1091</v>
@@ -39541,7 +39541,7 @@
     </row>
     <row r="262" spans="1:6">
       <c r="A262" t="s">
-        <v>760</v>
+        <v>526</v>
       </c>
       <c r="B262">
         <v>2401.777119828843</v>
@@ -39553,7 +39553,7 @@
         <v>1090</v>
       </c>
       <c r="E262">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F262" t="s">
         <v>1091</v>
@@ -39561,7 +39561,7 @@
     </row>
     <row r="263" spans="1:6">
       <c r="A263" t="s">
-        <v>526</v>
+        <v>717</v>
       </c>
       <c r="B263">
         <v>2401.777119828843</v>
@@ -39573,7 +39573,7 @@
         <v>1090</v>
       </c>
       <c r="E263">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F263" t="s">
         <v>1091</v>
@@ -39621,7 +39621,7 @@
     </row>
     <row r="266" spans="1:6">
       <c r="A266" t="s">
-        <v>527</v>
+        <v>789</v>
       </c>
       <c r="B266">
         <v>2401.777119828843</v>
@@ -39633,7 +39633,7 @@
         <v>1090</v>
       </c>
       <c r="E266">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F266" t="s">
         <v>1091</v>
@@ -39641,7 +39641,7 @@
     </row>
     <row r="267" spans="1:6">
       <c r="A267" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
       <c r="B267">
         <v>2401.777119828843</v>
@@ -39653,7 +39653,7 @@
         <v>1090</v>
       </c>
       <c r="E267">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F267" t="s">
         <v>1091</v>
@@ -39661,7 +39661,7 @@
     </row>
     <row r="268" spans="1:6">
       <c r="A268" t="s">
-        <v>772</v>
+        <v>527</v>
       </c>
       <c r="B268">
         <v>2401.777119828843</v>
@@ -39673,7 +39673,7 @@
         <v>1090</v>
       </c>
       <c r="E268">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F268" t="s">
         <v>1091</v>
@@ -39701,7 +39701,7 @@
     </row>
     <row r="270" spans="1:6">
       <c r="A270" t="s">
-        <v>718</v>
+        <v>761</v>
       </c>
       <c r="B270">
         <v>2401.777119828843</v>
@@ -39713,7 +39713,7 @@
         <v>1090</v>
       </c>
       <c r="E270">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F270" t="s">
         <v>1091</v>
@@ -39721,7 +39721,7 @@
     </row>
     <row r="271" spans="1:6">
       <c r="A271" t="s">
-        <v>761</v>
+        <v>678</v>
       </c>
       <c r="B271">
         <v>2401.777119828843</v>
@@ -39733,7 +39733,7 @@
         <v>1090</v>
       </c>
       <c r="E271">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F271" t="s">
         <v>1091</v>
@@ -39741,7 +39741,7 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" t="s">
-        <v>678</v>
+        <v>718</v>
       </c>
       <c r="B272">
         <v>2401.777119828843</v>
@@ -39753,7 +39753,7 @@
         <v>1090</v>
       </c>
       <c r="E272">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F272" t="s">
         <v>1091</v>
@@ -39761,7 +39761,7 @@
     </row>
     <row r="273" spans="1:6">
       <c r="A273" t="s">
-        <v>719</v>
+        <v>762</v>
       </c>
       <c r="B273">
         <v>2401.777119828843</v>
@@ -39773,7 +39773,7 @@
         <v>1090</v>
       </c>
       <c r="E273">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F273" t="s">
         <v>1091</v>
@@ -39781,7 +39781,7 @@
     </row>
     <row r="274" spans="1:6">
       <c r="A274" t="s">
-        <v>762</v>
+        <v>679</v>
       </c>
       <c r="B274">
         <v>2401.777119828843</v>
@@ -39793,7 +39793,7 @@
         <v>1090</v>
       </c>
       <c r="E274">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F274" t="s">
         <v>1091</v>
@@ -39801,7 +39801,7 @@
     </row>
     <row r="275" spans="1:6">
       <c r="A275" t="s">
-        <v>679</v>
+        <v>719</v>
       </c>
       <c r="B275">
         <v>2401.777119828843</v>
@@ -39813,7 +39813,7 @@
         <v>1090</v>
       </c>
       <c r="E275">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F275" t="s">
         <v>1091</v>
@@ -39821,7 +39821,7 @@
     </row>
     <row r="276" spans="1:6">
       <c r="A276" t="s">
-        <v>720</v>
+        <v>763</v>
       </c>
       <c r="B276">
         <v>2401.777119828843</v>
@@ -39833,7 +39833,7 @@
         <v>1090</v>
       </c>
       <c r="E276">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F276" t="s">
         <v>1091</v>
@@ -39841,7 +39841,7 @@
     </row>
     <row r="277" spans="1:6">
       <c r="A277" t="s">
-        <v>763</v>
+        <v>680</v>
       </c>
       <c r="B277">
         <v>2401.777119828843</v>
@@ -39853,7 +39853,7 @@
         <v>1090</v>
       </c>
       <c r="E277">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F277" t="s">
         <v>1091</v>
@@ -39861,7 +39861,7 @@
     </row>
     <row r="278" spans="1:6">
       <c r="A278" t="s">
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="B278">
         <v>2401.777119828843</v>
@@ -39873,7 +39873,7 @@
         <v>1090</v>
       </c>
       <c r="E278">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F278" t="s">
         <v>1091</v>
@@ -45103,7 +45103,7 @@
         <v>767</v>
       </c>
       <c r="B20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C20" t="s">
         <v>1113</v>
@@ -45117,7 +45117,7 @@
         <v>776</v>
       </c>
       <c r="B21" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="C21" t="s">
         <v>1114</v>
@@ -45131,7 +45131,7 @@
         <v>784</v>
       </c>
       <c r="B22" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C22" t="s">
         <v>1115</v>

</xml_diff>